<commit_message>
Initial commit with stroke analysis code
</commit_message>
<xml_diff>
--- a/results_full_strokes_A/stroke_phase_metrics.xlsx
+++ b/results_full_strokes_A/stroke_phase_metrics.xlsx
@@ -512,133 +512,133 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.85</v>
+        <v>0.875</v>
       </c>
       <c r="C2">
-        <v>0.691666666666667</v>
+        <v>0.791666666666667</v>
       </c>
       <c r="D2">
+        <v>0.7</v>
+      </c>
+      <c r="E2">
+        <v>0.683333333333333</v>
+      </c>
+      <c r="F2">
+        <v>0.608333333333333</v>
+      </c>
+      <c r="G2">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2">
+        <v>0.658333333333333</v>
+      </c>
+      <c r="I2">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J2">
+        <v>0.608333333333333</v>
+      </c>
+      <c r="K2">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="L2">
+        <v>0.608333333333333</v>
+      </c>
+      <c r="M2">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="N2">
+        <v>0.525</v>
+      </c>
+      <c r="O2">
+        <v>0.575</v>
+      </c>
+      <c r="P2">
         <v>0.591666666666667</v>
       </c>
-      <c r="E2">
-        <v>0.625</v>
-      </c>
-      <c r="F2">
-        <v>0.541666666666667</v>
-      </c>
-      <c r="G2">
-        <v>0.491666666666667</v>
-      </c>
-      <c r="H2">
-        <v>0.55</v>
-      </c>
-      <c r="I2">
+      <c r="Q2">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="R2">
+        <v>0.558333333333333</v>
+      </c>
+      <c r="S2">
+        <v>0.5</v>
+      </c>
+      <c r="T2">
+        <v>0.508333333333333</v>
+      </c>
+      <c r="U2">
+        <v>0.508333333333333</v>
+      </c>
+      <c r="V2">
+        <v>0.566666666666667</v>
+      </c>
+      <c r="W2">
+        <v>0.525</v>
+      </c>
+      <c r="X2">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="Y2">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="Z2">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="AA2">
+        <v>0.508333333333333</v>
+      </c>
+      <c r="AB2">
+        <v>0.483333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.5</v>
+      </c>
+      <c r="AD2">
+        <v>0.5</v>
+      </c>
+      <c r="AE2">
+        <v>0.475</v>
+      </c>
+      <c r="AF2">
         <v>0.466666666666667</v>
       </c>
-      <c r="J2">
-        <v>0.533333333333333</v>
-      </c>
-      <c r="K2">
-        <v>0.491666666666667</v>
-      </c>
-      <c r="L2">
-        <v>0.525</v>
-      </c>
-      <c r="M2">
-        <v>0.483333333333333</v>
-      </c>
-      <c r="N2">
+      <c r="AG2">
+        <v>0.441666666666667</v>
+      </c>
+      <c r="AH2">
+        <v>0.45</v>
+      </c>
+      <c r="AI2">
         <v>0.458333333333333</v>
       </c>
-      <c r="O2">
-        <v>0.508333333333333</v>
-      </c>
-      <c r="P2">
-        <v>0.508333333333333</v>
-      </c>
-      <c r="Q2">
+      <c r="AJ2">
+        <v>0.475</v>
+      </c>
+      <c r="AK2">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.45</v>
+      </c>
+      <c r="AM2">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="AN2">
+        <v>0.441666666666667</v>
+      </c>
+      <c r="AO2">
         <v>0.466666666666667</v>
       </c>
-      <c r="R2">
+      <c r="AP2">
         <v>0.466666666666667</v>
       </c>
-      <c r="S2">
+      <c r="AQ2">
+        <v>0.475</v>
+      </c>
+      <c r="AR2">
         <v>0.466666666666667</v>
-      </c>
-      <c r="T2">
-        <v>0.458333333333333</v>
-      </c>
-      <c r="U2">
-        <v>0.45</v>
-      </c>
-      <c r="V2">
-        <v>0.483333333333333</v>
-      </c>
-      <c r="W2">
-        <v>0.466666666666667</v>
-      </c>
-      <c r="X2">
-        <v>0.466666666666667</v>
-      </c>
-      <c r="Y2">
-        <v>0.441666666666667</v>
-      </c>
-      <c r="Z2">
-        <v>0.425</v>
-      </c>
-      <c r="AA2">
-        <v>0.441666666666667</v>
-      </c>
-      <c r="AB2">
-        <v>0.425</v>
-      </c>
-      <c r="AC2">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="AD2">
-        <v>0.425</v>
-      </c>
-      <c r="AE2">
-        <v>0.433333333333333</v>
-      </c>
-      <c r="AF2">
-        <v>0.425</v>
-      </c>
-      <c r="AG2">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="AH2">
-        <v>0.4</v>
-      </c>
-      <c r="AI2">
-        <v>0.408333333333333</v>
-      </c>
-      <c r="AJ2">
-        <v>0.425</v>
-      </c>
-      <c r="AK2">
-        <v>0.408333333333333</v>
-      </c>
-      <c r="AL2">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="AM2">
-        <v>0.383333333333333</v>
-      </c>
-      <c r="AN2">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="AO2">
-        <v>0.425</v>
-      </c>
-      <c r="AP2">
-        <v>0.433333333333333</v>
-      </c>
-      <c r="AQ2">
-        <v>0.425</v>
-      </c>
-      <c r="AR2">
-        <v>0.441666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:44">
@@ -646,133 +646,133 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.62658347365401</v>
+        <v>2.08769357026455</v>
       </c>
       <c r="C3">
-        <v>3.24383178275941</v>
+        <v>2.51854097451018</v>
       </c>
       <c r="D3">
-        <v>3.99080404755157</v>
+        <v>3.1228502003203</v>
       </c>
       <c r="E3">
-        <v>4.06863861812632</v>
+        <v>3.00144711843817</v>
       </c>
       <c r="F3">
-        <v>3.93709992054884</v>
+        <v>3.13339359040637</v>
       </c>
       <c r="G3">
-        <v>4.53492935978916</v>
+        <v>3.51398837216782</v>
       </c>
       <c r="H3">
-        <v>4.57965508235255</v>
+        <v>3.58142461188398</v>
       </c>
       <c r="I3">
-        <v>4.8627544496329</v>
+        <v>3.75191859848081</v>
       </c>
       <c r="J3">
-        <v>4.61056213796464</v>
+        <v>3.55717649392736</v>
       </c>
       <c r="K3">
-        <v>4.8212832419125</v>
+        <v>3.63489575761161</v>
       </c>
       <c r="L3">
-        <v>4.44173526366651</v>
+        <v>3.41002073412859</v>
       </c>
       <c r="M3">
-        <v>5.06699239166439</v>
+        <v>3.89593493788108</v>
       </c>
       <c r="N3">
-        <v>4.89512749674933</v>
+        <v>3.7691959511199</v>
       </c>
       <c r="O3">
-        <v>4.71771924935274</v>
+        <v>3.61579682127176</v>
       </c>
       <c r="P3">
-        <v>4.84464617849398</v>
+        <v>3.73374441216008</v>
       </c>
       <c r="Q3">
-        <v>5.51562506670867</v>
+        <v>4.26220828145275</v>
       </c>
       <c r="R3">
-        <v>5.0615841509777</v>
+        <v>3.8834090191933</v>
       </c>
       <c r="S3">
-        <v>5.26254003270689</v>
+        <v>4.07796162462167</v>
       </c>
       <c r="T3">
-        <v>5.25323535340851</v>
+        <v>4.0853975817954</v>
       </c>
       <c r="U3">
-        <v>5.3004423474396</v>
+        <v>4.0933310060099</v>
       </c>
       <c r="V3">
-        <v>5.55979939567221</v>
+        <v>4.15381729859521</v>
       </c>
       <c r="W3">
-        <v>5.24899030062831</v>
+        <v>4.05493092003647</v>
       </c>
       <c r="X3">
-        <v>5.26837687772645</v>
+        <v>4.10256235363165</v>
       </c>
       <c r="Y3">
-        <v>5.71057756619804</v>
+        <v>4.26544170785312</v>
       </c>
       <c r="Z3">
-        <v>6.10925625239688</v>
+        <v>4.6060708497253</v>
       </c>
       <c r="AA3">
-        <v>6.59368568318984</v>
+        <v>4.97120924123934</v>
       </c>
       <c r="AB3">
-        <v>6.60895372568185</v>
+        <v>5.06131920577455</v>
       </c>
       <c r="AC3">
-        <v>6.96987320327676</v>
+        <v>5.26060783981266</v>
       </c>
       <c r="AD3">
-        <v>7.12252896669515</v>
+        <v>5.33260664553444</v>
       </c>
       <c r="AE3">
-        <v>6.98607819026959</v>
+        <v>5.25578855652519</v>
       </c>
       <c r="AF3">
-        <v>7.09635269085184</v>
+        <v>5.36215819425034</v>
       </c>
       <c r="AG3">
-        <v>7.42063690261533</v>
+        <v>5.59313252057335</v>
       </c>
       <c r="AH3">
-        <v>7.11215222575537</v>
+        <v>5.41512135029575</v>
       </c>
       <c r="AI3">
-        <v>7.23658009940996</v>
+        <v>5.44361274591991</v>
       </c>
       <c r="AJ3">
-        <v>7.36641136429875</v>
+        <v>5.50902516743148</v>
       </c>
       <c r="AK3">
-        <v>7.52712566475038</v>
+        <v>5.59490420371929</v>
       </c>
       <c r="AL3">
-        <v>7.2521215134221</v>
+        <v>5.39965607335965</v>
       </c>
       <c r="AM3">
-        <v>7.20994192600496</v>
+        <v>5.49135706870043</v>
       </c>
       <c r="AN3">
-        <v>7.54894328676226</v>
+        <v>5.50087463080083</v>
       </c>
       <c r="AO3">
-        <v>7.32509172401868</v>
+        <v>5.64072656213329</v>
       </c>
       <c r="AP3">
-        <v>7.3094116763726</v>
+        <v>5.61813065244701</v>
       </c>
       <c r="AQ3">
-        <v>7.17190464986271</v>
+        <v>5.60015474746013</v>
       </c>
       <c r="AR3">
-        <v>7.27269942130979</v>
+        <v>5.56073849712864</v>
       </c>
     </row>
     <row r="4" spans="1:44">
@@ -780,133 +780,133 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>31.3725490196078</v>
+        <v>35.2380952380952</v>
       </c>
       <c r="C4">
-        <v>38.5542168674699</v>
+        <v>31.5789473684211</v>
       </c>
       <c r="D4">
-        <v>42.2535211267606</v>
+        <v>36.9047619047619</v>
       </c>
       <c r="E4">
-        <v>33.3333333333333</v>
+        <v>32.9268292682927</v>
       </c>
       <c r="F4">
+        <v>42.4657534246575</v>
+      </c>
+      <c r="G4">
+        <v>41.4285714285714</v>
+      </c>
+      <c r="H4">
+        <v>39.2405063291139</v>
+      </c>
+      <c r="I4">
+        <v>48.4375</v>
+      </c>
+      <c r="J4">
+        <v>42.4657534246575</v>
+      </c>
+      <c r="K4">
         <v>46.1538461538462</v>
       </c>
-      <c r="G4">
-        <v>42.3728813559322</v>
-      </c>
-      <c r="H4">
-        <v>48.4848484848485</v>
-      </c>
-      <c r="I4">
+      <c r="L4">
+        <v>43.8356164383562</v>
+      </c>
+      <c r="M4">
+        <v>44.6153846153846</v>
+      </c>
+      <c r="N4">
+        <v>46.031746031746</v>
+      </c>
+      <c r="O4">
+        <v>44.9275362318841</v>
+      </c>
+      <c r="P4">
+        <v>43.6619718309859</v>
+      </c>
+      <c r="Q4">
+        <v>46.875</v>
+      </c>
+      <c r="R4">
+        <v>41.7910447761194</v>
+      </c>
+      <c r="S4">
         <v>50</v>
       </c>
-      <c r="J4">
-        <v>51.5625</v>
-      </c>
-      <c r="K4">
-        <v>50.8474576271186</v>
-      </c>
-      <c r="L4">
-        <v>53.968253968254</v>
-      </c>
-      <c r="M4">
+      <c r="T4">
+        <v>49.1803278688525</v>
+      </c>
+      <c r="U4">
+        <v>45.9016393442623</v>
+      </c>
+      <c r="V4">
+        <v>39.7058823529412</v>
+      </c>
+      <c r="W4">
+        <v>46.031746031746</v>
+      </c>
+      <c r="X4">
+        <v>48.4375</v>
+      </c>
+      <c r="Y4">
+        <v>43.75</v>
+      </c>
+      <c r="Z4">
+        <v>43.75</v>
+      </c>
+      <c r="AA4">
+        <v>45.9016393442623</v>
+      </c>
+      <c r="AB4">
+        <v>48.2758620689655</v>
+      </c>
+      <c r="AC4">
+        <v>43.3333333333333</v>
+      </c>
+      <c r="AD4">
+        <v>43.3333333333333</v>
+      </c>
+      <c r="AE4">
+        <v>45.6140350877193</v>
+      </c>
+      <c r="AF4">
         <v>50</v>
       </c>
-      <c r="N4">
-        <v>50.9090909090909</v>
-      </c>
-      <c r="O4">
-        <v>52.4590163934426</v>
-      </c>
-      <c r="P4">
-        <v>50.8196721311476</v>
-      </c>
-      <c r="Q4">
-        <v>55.3571428571429</v>
-      </c>
-      <c r="R4">
-        <v>48.2142857142857</v>
-      </c>
-      <c r="S4">
+      <c r="AG4">
+        <v>49.0566037735849</v>
+      </c>
+      <c r="AH4">
+        <v>46.2962962962963</v>
+      </c>
+      <c r="AI4">
+        <v>47.2727272727273</v>
+      </c>
+      <c r="AJ4">
+        <v>45.6140350877193</v>
+      </c>
+      <c r="AK4">
+        <v>47.2727272727273</v>
+      </c>
+      <c r="AL4">
+        <v>48.1481481481482</v>
+      </c>
+      <c r="AM4">
+        <v>47.2727272727273</v>
+      </c>
+      <c r="AN4">
+        <v>49.0566037735849</v>
+      </c>
+      <c r="AO4">
         <v>53.5714285714286</v>
       </c>
-      <c r="T4">
-        <v>54.5454545454546</v>
-      </c>
-      <c r="U4">
-        <v>51.8518518518518</v>
-      </c>
-      <c r="V4">
-        <v>48.2758620689655</v>
-      </c>
-      <c r="W4">
-        <v>50</v>
-      </c>
-      <c r="X4">
-        <v>53.5714285714286</v>
-      </c>
-      <c r="Y4">
-        <v>50.9433962264151</v>
-      </c>
-      <c r="Z4">
-        <v>54.9019607843137</v>
-      </c>
-      <c r="AA4">
-        <v>52.8301886792453</v>
-      </c>
-      <c r="AB4">
-        <v>56.8627450980392</v>
-      </c>
-      <c r="AC4">
-        <v>46</v>
-      </c>
-      <c r="AD4">
-        <v>54.9019607843137</v>
-      </c>
-      <c r="AE4">
-        <v>50</v>
-      </c>
-      <c r="AF4">
-        <v>58.8235294117647</v>
-      </c>
-      <c r="AG4">
-        <v>54</v>
-      </c>
-      <c r="AH4">
-        <v>54.1666666666667</v>
-      </c>
-      <c r="AI4">
-        <v>53.0612244897959</v>
-      </c>
-      <c r="AJ4">
-        <v>56.8627450980392</v>
-      </c>
-      <c r="AK4">
-        <v>57.1428571428571</v>
-      </c>
-      <c r="AL4">
-        <v>54</v>
-      </c>
-      <c r="AM4">
-        <v>56.5217391304348</v>
-      </c>
-      <c r="AN4">
-        <v>54</v>
-      </c>
-      <c r="AO4">
-        <v>60.7843137254902</v>
-      </c>
       <c r="AP4">
-        <v>55.7692307692308</v>
+        <v>51.7857142857143</v>
       </c>
       <c r="AQ4">
-        <v>64.7058823529412</v>
+        <v>52.6315789473684</v>
       </c>
       <c r="AR4">
-        <v>52.8301886792453</v>
+        <v>51.7857142857143</v>
       </c>
     </row>
     <row r="5" spans="1:44">
@@ -914,133 +914,133 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>9.84968802620255</v>
+        <v>6.77089806572288</v>
       </c>
       <c r="C5">
-        <v>12.1643691853478</v>
+        <v>10.0741638980407</v>
       </c>
       <c r="D5">
-        <v>15.9632161902063</v>
+        <v>12.0884523883366</v>
       </c>
       <c r="E5">
-        <v>19.5294653670063</v>
+        <v>13.3397649708363</v>
       </c>
       <c r="F5">
-        <v>15.7483996821954</v>
+        <v>12.1292655112504</v>
       </c>
       <c r="G5">
-        <v>21.767660926988</v>
+        <v>14.5406415400048</v>
       </c>
       <c r="H5">
-        <v>17.1737065588221</v>
+        <v>13.8635791427767</v>
       </c>
       <c r="I5">
-        <v>20.8403762127124</v>
+        <v>14.523555865087</v>
       </c>
       <c r="J5">
-        <v>16.7656805016896</v>
+        <v>13.769715460364</v>
       </c>
       <c r="K5">
-        <v>19.28513296765</v>
+        <v>14.5395830304464</v>
       </c>
       <c r="L5">
-        <v>15.6767126952936</v>
+        <v>12.7875777529822</v>
       </c>
       <c r="M5">
-        <v>20.9668650689561</v>
+        <v>16.1211100877838</v>
       </c>
       <c r="N5">
-        <v>20.9791178432114</v>
+        <v>15.5966729011858</v>
       </c>
       <c r="O5">
-        <v>17.6914471850728</v>
+        <v>13.9966328565358</v>
       </c>
       <c r="P5">
-        <v>18.7534690780412</v>
+        <v>14.4532041761035</v>
       </c>
       <c r="Q5">
-        <v>21.35080670984</v>
+        <v>17.048833125811</v>
       </c>
       <c r="R5">
-        <v>22.4959295599009</v>
+        <v>16.6431815108284</v>
       </c>
       <c r="S5">
-        <v>21.0501601308276</v>
+        <v>16.3118464984867</v>
       </c>
       <c r="T5">
-        <v>21.012941413634</v>
+        <v>16.3415903271816</v>
       </c>
       <c r="U5">
-        <v>22.7161814890268</v>
+        <v>17.5428471686138</v>
       </c>
       <c r="V5">
-        <v>23.827711695738</v>
+        <v>18.4614102159787</v>
       </c>
       <c r="W5">
-        <v>22.4956727169785</v>
+        <v>16.7790244967026</v>
       </c>
       <c r="X5">
-        <v>21.0735075109058</v>
+        <v>15.880886530187</v>
       </c>
       <c r="Y5">
-        <v>25.380344738658</v>
+        <v>18.2804644622277</v>
       </c>
       <c r="Z5">
-        <v>26.1825267959866</v>
+        <v>19.7403036416799</v>
       </c>
       <c r="AA5">
-        <v>28.2586529279564</v>
+        <v>21.3051824624543</v>
       </c>
       <c r="AB5">
-        <v>27.3473947269594</v>
+        <v>21.6913680247481</v>
       </c>
       <c r="AC5">
-        <v>36.3645558431831</v>
+        <v>24.279728491443</v>
       </c>
       <c r="AD5">
-        <v>30.5251241429792</v>
+        <v>24.6120306716974</v>
       </c>
       <c r="AE5">
-        <v>32.2434378012443</v>
+        <v>24.2574856455009</v>
       </c>
       <c r="AF5">
-        <v>28.3854107634074</v>
+        <v>22.9806779753586</v>
       </c>
       <c r="AG5">
-        <v>32.9806084560681</v>
+        <v>25.8144577872616</v>
       </c>
       <c r="AH5">
-        <v>32.8253179650248</v>
+        <v>25.9925824814196</v>
       </c>
       <c r="AI5">
-        <v>33.3996004588152</v>
+        <v>25.1243665196304</v>
       </c>
       <c r="AJ5">
-        <v>30.4817021970983</v>
+        <v>25.4262700035299</v>
       </c>
       <c r="AK5">
-        <v>32.2591099917873</v>
+        <v>25.8226347863967</v>
       </c>
       <c r="AL5">
-        <v>32.2316511707649</v>
+        <v>24.9214895693522</v>
       </c>
       <c r="AM5">
-        <v>33.2766550430998</v>
+        <v>25.3447249324635</v>
       </c>
       <c r="AN5">
-        <v>33.5508590522767</v>
+        <v>25.3886521421577</v>
       </c>
       <c r="AO5">
-        <v>28.3551937703949</v>
+        <v>22.5629062485331</v>
       </c>
       <c r="AP5">
-        <v>30.2458414194728</v>
+        <v>23.2474371825393</v>
       </c>
       <c r="AQ5">
-        <v>26.0796532722281</v>
+        <v>22.4006189898405</v>
       </c>
       <c r="AR5">
-        <v>31.1687118056134</v>
+        <v>23.0099524019116</v>
       </c>
     </row>
     <row r="6" spans="1:44">
@@ -1048,133 +1048,133 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1.29684559748837</v>
+        <v>1.17464255919758</v>
       </c>
       <c r="C6">
-        <v>1.13478498681825</v>
+        <v>1.02315831196418</v>
       </c>
       <c r="D6">
-        <v>1.29161984713098</v>
+        <v>1.1594235859966</v>
       </c>
       <c r="E6">
-        <v>1.25251764833907</v>
+        <v>1.10390328131061</v>
       </c>
       <c r="F6">
-        <v>1.25994395198104</v>
+        <v>1.07960473987232</v>
       </c>
       <c r="G6">
-        <v>1.30058147869491</v>
+        <v>1.10971059864543</v>
       </c>
       <c r="H6">
-        <v>1.35195940734963</v>
+        <v>1.18313401747381</v>
       </c>
       <c r="I6">
-        <v>1.35876993113986</v>
+        <v>1.12964978526622</v>
       </c>
       <c r="J6">
-        <v>1.31489664683088</v>
+        <v>1.11893505403933</v>
       </c>
       <c r="K6">
-        <v>1.30531991827592</v>
+        <v>1.081171481432</v>
       </c>
       <c r="L6">
-        <v>1.22086934933015</v>
+        <v>1.05007683241595</v>
       </c>
       <c r="M6">
-        <v>1.38760818607725</v>
+        <v>1.15529105724065</v>
       </c>
       <c r="N6">
-        <v>1.30163735701186</v>
+        <v>1.0877399360589</v>
       </c>
       <c r="O6">
-        <v>1.28088402688073</v>
+        <v>1.08475749876894</v>
       </c>
       <c r="P6">
-        <v>1.30266126250612</v>
+        <v>1.11864248282318</v>
       </c>
       <c r="Q6">
-        <v>1.46892411581522</v>
+        <v>1.21951093358973</v>
       </c>
       <c r="R6">
-        <v>1.40349163208406</v>
+        <v>1.18008366399453</v>
       </c>
       <c r="S6">
-        <v>1.44862502066774</v>
+        <v>1.17628527723652</v>
       </c>
       <c r="T6">
-        <v>1.40519844746279</v>
+        <v>1.15857959277291</v>
       </c>
       <c r="U6">
-        <v>1.42418129427971</v>
+        <v>1.16203060269749</v>
       </c>
       <c r="V6">
-        <v>1.48147940207701</v>
+        <v>1.24520142986059</v>
       </c>
       <c r="W6">
-        <v>1.4368189983463</v>
+        <v>1.19524644046184</v>
       </c>
       <c r="X6">
-        <v>1.40527865598203</v>
+        <v>1.16773041135413</v>
       </c>
       <c r="Y6">
-        <v>1.43929395796719</v>
+        <v>1.18465190321815</v>
       </c>
       <c r="Z6">
-        <v>1.47122711259549</v>
+        <v>1.20053328704348</v>
       </c>
       <c r="AA6">
-        <v>1.63685227453024</v>
+        <v>1.3373391660269</v>
       </c>
       <c r="AB6">
-        <v>1.61426626386361</v>
+        <v>1.30870751933255</v>
       </c>
       <c r="AC6">
-        <v>1.7331360468804</v>
+        <v>1.41619465626306</v>
       </c>
       <c r="AD6">
-        <v>1.69643929291141</v>
+        <v>1.36654702103403</v>
       </c>
       <c r="AE6">
-        <v>1.7349498219996</v>
+        <v>1.39358767998284</v>
       </c>
       <c r="AF6">
-        <v>1.75787025286189</v>
+        <v>1.383970387249</v>
       </c>
       <c r="AG6">
-        <v>1.85787615790715</v>
+        <v>1.44073662365084</v>
       </c>
       <c r="AH6">
-        <v>1.79890852637617</v>
+        <v>1.40995120074443</v>
       </c>
       <c r="AI6">
-        <v>1.76501582348174</v>
+        <v>1.3732179902427</v>
       </c>
       <c r="AJ6">
-        <v>1.7516127583704</v>
+        <v>1.38596409035177</v>
       </c>
       <c r="AK6">
-        <v>1.792180275983</v>
+        <v>1.40058879030689</v>
       </c>
       <c r="AL6">
-        <v>1.74939410010772</v>
+        <v>1.38085997678907</v>
       </c>
       <c r="AM6">
-        <v>1.7638605580986</v>
+        <v>1.37197614769332</v>
       </c>
       <c r="AN6">
-        <v>1.781467465452</v>
+        <v>1.35934480452395</v>
       </c>
       <c r="AO6">
-        <v>1.86113235467867</v>
+        <v>1.43656943671564</v>
       </c>
       <c r="AP6">
-        <v>1.90755317238178</v>
+        <v>1.48516469902386</v>
       </c>
       <c r="AQ6">
-        <v>1.83123398246933</v>
+        <v>1.4260184371806</v>
       </c>
       <c r="AR6">
-        <v>1.90345015303705</v>
+        <v>1.48910587681186</v>
       </c>
     </row>
     <row r="7" spans="1:44">
@@ -1182,133 +1182,133 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.107175475247525</v>
+        <v>0.113620528846154</v>
       </c>
       <c r="C7">
-        <v>0.155205663414634</v>
+        <v>0.140069727659575</v>
       </c>
       <c r="D7">
-        <v>0.116130185714286</v>
+        <v>0.120392826506024</v>
       </c>
       <c r="E7">
-        <v>0.115734243243243</v>
+        <v>0.129262580246914</v>
       </c>
       <c r="F7">
-        <v>0.20929640625</v>
+        <v>0.213945580555555</v>
       </c>
       <c r="G7">
-        <v>0.12578225862069</v>
+        <v>0.128067056521739</v>
       </c>
       <c r="H7">
-        <v>0.229272769230769</v>
+        <v>0.20903017948718</v>
       </c>
       <c r="I7">
-        <v>0.181888545454545</v>
+        <v>0.180127984126984</v>
       </c>
       <c r="J7">
-        <v>0.178260444444444</v>
+        <v>0.183626527777778</v>
       </c>
       <c r="K7">
-        <v>0.220486379310345</v>
+        <v>0.229439890625</v>
       </c>
       <c r="L7">
-        <v>0.149795693548387</v>
+        <v>0.1343085</v>
       </c>
       <c r="M7">
-        <v>0.170359157894737</v>
+        <v>0.153894365625</v>
       </c>
       <c r="N7">
-        <v>0.179383092592593</v>
+        <v>0.167827838709677</v>
       </c>
       <c r="O7">
-        <v>0.138422083333333</v>
+        <v>0.148097897058824</v>
       </c>
       <c r="P7">
-        <v>0.18282725</v>
+        <v>0.165352314285714</v>
       </c>
       <c r="Q7">
-        <v>0.1536456</v>
+        <v>0.138110222222222</v>
       </c>
       <c r="R7">
-        <v>0.0949512727272727</v>
+        <v>0.0918066666666666</v>
       </c>
       <c r="S7">
-        <v>0.168125345454546</v>
+        <v>0.149451152542373</v>
       </c>
       <c r="T7">
-        <v>0.123523555555556</v>
+        <v>0.125694236666667</v>
       </c>
       <c r="U7">
-        <v>0.220115698113208</v>
+        <v>0.2102532</v>
       </c>
       <c r="V7">
-        <v>0.186473578947368</v>
+        <v>0.195475328358209</v>
       </c>
       <c r="W7">
-        <v>0.202841581818182</v>
+        <v>0.181394548387097</v>
       </c>
       <c r="X7">
-        <v>0.226616363636364</v>
+        <v>0.214278492063492</v>
       </c>
       <c r="Y7">
-        <v>0.237707442307692</v>
+        <v>0.212600174603175</v>
       </c>
       <c r="Z7">
-        <v>0.16940636</v>
+        <v>0.152549825396825</v>
       </c>
       <c r="AA7">
-        <v>0.460452884615385</v>
+        <v>0.39973485</v>
       </c>
       <c r="AB7">
-        <v>0.3670172</v>
+        <v>0.340003719298246</v>
       </c>
       <c r="AC7">
-        <v>0.365146265306122</v>
+        <v>0.285705305084746</v>
       </c>
       <c r="AD7">
-        <v>0.42795808</v>
+        <v>0.389668644067797</v>
       </c>
       <c r="AE7">
-        <v>0.343457019607843</v>
+        <v>0.307609107142857</v>
       </c>
       <c r="AF7">
-        <v>0.26706232</v>
+        <v>0.269412109090909</v>
       </c>
       <c r="AG7">
-        <v>0.332814326530612</v>
+        <v>0.327717211538462</v>
       </c>
       <c r="AH7">
-        <v>0.134888170212766</v>
+        <v>0.15027358490566</v>
       </c>
       <c r="AI7">
-        <v>0.498786041666667</v>
+        <v>0.468171240740741</v>
       </c>
       <c r="AJ7">
-        <v>0.30282722</v>
+        <v>0.28620875</v>
       </c>
       <c r="AK7">
-        <v>0.301122854166667</v>
+        <v>0.329286388888889</v>
       </c>
       <c r="AL7">
-        <v>0.450376163265306</v>
+        <v>0.454802981132076</v>
       </c>
       <c r="AM7">
-        <v>0.368458177777778</v>
+        <v>0.349750216666667</v>
       </c>
       <c r="AN7">
-        <v>0.212746877551021</v>
+        <v>0.204530819230769</v>
       </c>
       <c r="AO7">
-        <v>0.31746232</v>
+        <v>0.284389145454545</v>
       </c>
       <c r="AP7">
-        <v>0.399612745098039</v>
+        <v>0.363879272727273</v>
       </c>
       <c r="AQ7">
-        <v>0.30631258</v>
+        <v>0.258299071428571</v>
       </c>
       <c r="AR7">
-        <v>0.292131019230769</v>
+        <v>0.268456363636364</v>
       </c>
     </row>
     <row r="8" spans="1:44">
@@ -1316,133 +1316,133 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.0372714752475248</v>
+        <v>0.0325043173076923</v>
       </c>
       <c r="C8">
-        <v>0.112795731707317</v>
+        <v>0.110749936170213</v>
       </c>
       <c r="D8">
-        <v>0.172177628571429</v>
+        <v>0.171946722891566</v>
       </c>
       <c r="E8">
-        <v>0.26039027027027</v>
+        <v>0.243586419753086</v>
       </c>
       <c r="F8">
-        <v>0.2454284375</v>
+        <v>0.263577777777778</v>
       </c>
       <c r="G8">
-        <v>0.280712068965517</v>
+        <v>0.320351594202899</v>
       </c>
       <c r="H8">
-        <v>0.260376461538462</v>
+        <v>0.284709358974359</v>
       </c>
       <c r="I8">
-        <v>0.265169818181818</v>
+        <v>0.322018888888889</v>
       </c>
       <c r="J8">
-        <v>0.232680476190476</v>
+        <v>0.289148611111111</v>
       </c>
       <c r="K8">
-        <v>0.24056724137931</v>
+        <v>0.290639375</v>
       </c>
       <c r="L8">
-        <v>0.203632258064516</v>
+        <v>0.263757111111111</v>
       </c>
       <c r="M8">
-        <v>0.258098245614035</v>
+        <v>0.30030578125</v>
       </c>
       <c r="N8">
-        <v>0.244683148148148</v>
+        <v>0.296409032258065</v>
       </c>
       <c r="O8">
-        <v>0.275312666666667</v>
+        <v>0.334058882352941</v>
       </c>
       <c r="P8">
-        <v>0.252800833333333</v>
+        <v>0.315932142857143</v>
       </c>
       <c r="Q8">
-        <v>0.266935272727273</v>
+        <v>0.316704603174603</v>
       </c>
       <c r="R8">
-        <v>0.279066727272727</v>
+        <v>0.333850393939394</v>
       </c>
       <c r="S8">
-        <v>0.241146727272727</v>
+        <v>0.277250677966102</v>
       </c>
       <c r="T8">
-        <v>0.26429</v>
+        <v>0.3173575</v>
       </c>
       <c r="U8">
-        <v>0.227490566037736</v>
+        <v>0.2849025</v>
       </c>
       <c r="V8">
-        <v>0.263612456140351</v>
+        <v>0.320921820895522</v>
       </c>
       <c r="W8">
-        <v>0.285181454545455</v>
+        <v>0.341118548387097</v>
       </c>
       <c r="X8">
-        <v>0.265055090909091</v>
+        <v>0.312967619047619</v>
       </c>
       <c r="Y8">
-        <v>0.291247884615385</v>
+        <v>0.343893428571429</v>
       </c>
       <c r="Z8">
-        <v>0.3073022</v>
+        <v>0.355609206349206</v>
       </c>
       <c r="AA8">
-        <v>0.349574423076923</v>
+        <v>0.395640833333333</v>
       </c>
       <c r="AB8">
-        <v>0.3142678</v>
+        <v>0.345500350877193</v>
       </c>
       <c r="AC8">
-        <v>0.323789795918367</v>
+        <v>0.363864237288136</v>
       </c>
       <c r="AD8">
-        <v>0.3689058</v>
+        <v>0.396411186440678</v>
       </c>
       <c r="AE8">
-        <v>0.389131568627451</v>
+        <v>0.38651625</v>
       </c>
       <c r="AF8">
-        <v>0.4295184</v>
+        <v>0.391736</v>
       </c>
       <c r="AG8">
-        <v>0.491730755102041</v>
+        <v>0.424617115384615</v>
       </c>
       <c r="AH8">
-        <v>0.442903957446809</v>
+        <v>0.364159433962264</v>
       </c>
       <c r="AI8">
-        <v>0.37791625</v>
+        <v>0.360000740740741</v>
       </c>
       <c r="AJ8">
-        <v>0.374736</v>
+        <v>0.357809464285714</v>
       </c>
       <c r="AK8">
-        <v>0.428684041666667</v>
+        <v>0.36352</v>
       </c>
       <c r="AL8">
-        <v>0.383064632653061</v>
+        <v>0.351122452830189</v>
       </c>
       <c r="AM8">
-        <v>0.416148733333333</v>
+        <v>0.350386296296296</v>
       </c>
       <c r="AN8">
-        <v>0.416288571428571</v>
+        <v>0.378609615384616</v>
       </c>
       <c r="AO8">
-        <v>0.4402758</v>
+        <v>0.368594909090909</v>
       </c>
       <c r="AP8">
-        <v>0.396695490196078</v>
+        <v>0.339522909090909</v>
       </c>
       <c r="AQ8">
-        <v>0.39265826</v>
+        <v>0.346158214285714</v>
       </c>
       <c r="AR8">
-        <v>0.343195384615385</v>
+        <v>0.314102</v>
       </c>
     </row>
     <row r="9" spans="1:44">
@@ -1450,133 +1450,133 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.04230589108911</v>
+        <v>1.19899634615385</v>
       </c>
       <c r="C9">
-        <v>1.73451156097561</v>
+        <v>1.72890627659575</v>
       </c>
       <c r="D9">
-        <v>1.36826371428571</v>
+        <v>1.29423481927711</v>
       </c>
       <c r="E9">
-        <v>1.21264635135135</v>
+        <v>1.14008592592593</v>
       </c>
       <c r="F9">
-        <v>2.97250125</v>
+        <v>2.69573194444444</v>
       </c>
       <c r="G9">
-        <v>1.18089724137931</v>
+        <v>1.2476668115942</v>
       </c>
       <c r="H9">
-        <v>2.22879476923077</v>
+        <v>2.02389871794872</v>
       </c>
       <c r="I9">
-        <v>2.18694707272727</v>
+        <v>2.00396619047619</v>
       </c>
       <c r="J9">
-        <v>2.06861587301587</v>
+        <v>2.15272986111111</v>
       </c>
       <c r="K9">
-        <v>1.91422896551724</v>
+        <v>2.043221875</v>
       </c>
       <c r="L9">
-        <v>1.32064225806452</v>
+        <v>1.15468458333333</v>
       </c>
       <c r="M9">
-        <v>1.76776659649123</v>
+        <v>1.47375609375</v>
       </c>
       <c r="N9">
-        <v>2.56162792222222</v>
+        <v>2.222225</v>
       </c>
       <c r="O9">
-        <v>1.30020538333333</v>
+        <v>1.33469882352941</v>
       </c>
       <c r="P9">
-        <v>2.45760616666667</v>
+        <v>2.04882428571429</v>
       </c>
       <c r="Q9">
-        <v>2.31057272727273</v>
+        <v>2.04347901587302</v>
       </c>
       <c r="R9">
-        <v>1.34943745454545</v>
+        <v>1.21984333333333</v>
       </c>
       <c r="S9">
-        <v>2.07724181818182</v>
+        <v>1.89458271186441</v>
       </c>
       <c r="T9">
-        <v>1.03467107407407</v>
+        <v>1.03082913333333</v>
       </c>
       <c r="U9">
-        <v>2.78201981132075</v>
+        <v>2.44855633333333</v>
       </c>
       <c r="V9">
-        <v>1.97034105263158</v>
+        <v>1.94743134328358</v>
       </c>
       <c r="W9">
-        <v>2.21086236363636</v>
+        <v>2.06992419354839</v>
       </c>
       <c r="X9">
-        <v>2.86917345454545</v>
+        <v>2.47121650793651</v>
       </c>
       <c r="Y9">
-        <v>2.18864157692308</v>
+        <v>1.760994</v>
       </c>
       <c r="Z9">
-        <v>1.661502</v>
+        <v>1.49639238095238</v>
       </c>
       <c r="AA9">
-        <v>5.1863675</v>
+        <v>4.66035666666667</v>
       </c>
       <c r="AB9">
-        <v>3.50108414</v>
+        <v>3.12617649122807</v>
       </c>
       <c r="AC9">
-        <v>3.63812046938775</v>
+        <v>2.97686610169491</v>
       </c>
       <c r="AD9">
-        <v>4.605816</v>
+        <v>4.89114101694915</v>
       </c>
       <c r="AE9">
-        <v>3.63601705882353</v>
+        <v>3.10299732142857</v>
       </c>
       <c r="AF9">
-        <v>3.53013</v>
+        <v>2.99255581818182</v>
       </c>
       <c r="AG9">
-        <v>3.64340234693878</v>
+        <v>3.31265615384615</v>
       </c>
       <c r="AH9">
-        <v>1.7549570212766</v>
+        <v>1.37069396226415</v>
       </c>
       <c r="AI9">
-        <v>5.47226875</v>
+        <v>4.86071851851852</v>
       </c>
       <c r="AJ9">
-        <v>3.530766</v>
+        <v>3.46136964285714</v>
       </c>
       <c r="AK9">
-        <v>2.84990520833333</v>
+        <v>2.69200833333333</v>
       </c>
       <c r="AL9">
-        <v>3.80440428571429</v>
+        <v>3.01195339622641</v>
       </c>
       <c r="AM9">
-        <v>3.6623</v>
+        <v>2.8700267962963</v>
       </c>
       <c r="AN9">
-        <v>1.84793867346939</v>
+        <v>1.54156384615385</v>
       </c>
       <c r="AO9">
-        <v>3.617836</v>
+        <v>2.81568636363636</v>
       </c>
       <c r="AP9">
-        <v>4.60265803921569</v>
+        <v>4.18110181818182</v>
       </c>
       <c r="AQ9">
-        <v>3.5761696</v>
+        <v>2.69799267857143</v>
       </c>
       <c r="AR9">
-        <v>3.44709480769231</v>
+        <v>3.22491218181818</v>
       </c>
     </row>
     <row r="10" spans="1:44">
@@ -1584,133 +1584,133 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.0593662277227723</v>
+        <v>0.061617375</v>
       </c>
       <c r="C10">
-        <v>0.0667690243902439</v>
+        <v>0.0587861595744681</v>
       </c>
       <c r="D10">
-        <v>0.0715857</v>
+        <v>0.0800989638554217</v>
       </c>
       <c r="E10">
-        <v>0.0740956486486486</v>
+        <v>0.0710071111111111</v>
       </c>
       <c r="F10">
-        <v>0.08729025</v>
+        <v>0.0813207222222222</v>
       </c>
       <c r="G10">
-        <v>0.0595728275862069</v>
+        <v>0.052628015942029</v>
       </c>
       <c r="H10">
-        <v>0.0567669538461539</v>
+        <v>0.0509791794871795</v>
       </c>
       <c r="I10">
-        <v>0.0831271818181818</v>
+        <v>0.0782529523809524</v>
       </c>
       <c r="J10">
-        <v>0.0950022222222222</v>
+        <v>0.0915942916666666</v>
       </c>
       <c r="K10">
-        <v>0.0647242068965517</v>
+        <v>0.07035659375</v>
       </c>
       <c r="L10">
-        <v>0.0666690967741935</v>
+        <v>0.0575013888888889</v>
       </c>
       <c r="M10">
-        <v>0.0623347368421053</v>
+        <v>0.060015625</v>
       </c>
       <c r="N10">
-        <v>0.0644466296296296</v>
+        <v>0.0617421612903226</v>
       </c>
       <c r="O10">
-        <v>0.0803830333333333</v>
+        <v>0.079409</v>
       </c>
       <c r="P10">
-        <v>0.103879783333333</v>
+        <v>0.0903144142857143</v>
       </c>
       <c r="Q10">
-        <v>0.0766463454545454</v>
+        <v>0.0701921428571428</v>
       </c>
       <c r="R10">
-        <v>0.0978052418181818</v>
+        <v>0.0852186515151515</v>
       </c>
       <c r="S10">
-        <v>0.0845222</v>
+        <v>0.0782963525423729</v>
       </c>
       <c r="T10">
-        <v>0.0683987037037037</v>
+        <v>0.0640386928333333</v>
       </c>
       <c r="U10">
-        <v>0.0973998490566038</v>
+        <v>0.0885775666666667</v>
       </c>
       <c r="V10">
-        <v>0.124893964912281</v>
+        <v>0.136225402985075</v>
       </c>
       <c r="W10">
-        <v>0.0803501818181818</v>
+        <v>0.0709000322580645</v>
       </c>
       <c r="X10">
-        <v>0.0876088727272727</v>
+        <v>0.080478</v>
       </c>
       <c r="Y10">
-        <v>0.0719907884615385</v>
+        <v>0.0644037619047619</v>
       </c>
       <c r="Z10">
-        <v>0.0654788</v>
+        <v>0.0524789682539683</v>
       </c>
       <c r="AA10">
-        <v>0.125241430769231</v>
+        <v>0.132615373333333</v>
       </c>
       <c r="AB10">
-        <v>0.101894</v>
+        <v>0.0879159122807018</v>
       </c>
       <c r="AC10">
-        <v>0.109331795918367</v>
+        <v>0.103476542372881</v>
       </c>
       <c r="AD10">
-        <v>0.11628232</v>
+        <v>0.11347119661017</v>
       </c>
       <c r="AE10">
-        <v>0.0763950980392157</v>
+        <v>0.0803876785714286</v>
       </c>
       <c r="AF10">
-        <v>0.1075688</v>
+        <v>0.115410727272727</v>
       </c>
       <c r="AG10">
-        <v>0.126194444897959</v>
+        <v>0.125670015384615</v>
       </c>
       <c r="AH10">
-        <v>0.105816191489362</v>
+        <v>0.0803339622641509</v>
       </c>
       <c r="AI10">
-        <v>0.137094333333333</v>
+        <v>0.113551388888889</v>
       </c>
       <c r="AJ10">
-        <v>0.1251746</v>
+        <v>0.12670875</v>
       </c>
       <c r="AK10">
-        <v>0.1508214375</v>
+        <v>0.13803562962963</v>
       </c>
       <c r="AL10">
-        <v>0.205313244897959</v>
+        <v>0.232543698113208</v>
       </c>
       <c r="AM10">
-        <v>0.1576914</v>
+        <v>0.172944240740741</v>
       </c>
       <c r="AN10">
-        <v>0.10888</v>
+        <v>0.106757173076923</v>
       </c>
       <c r="AO10">
-        <v>0.0910766</v>
+        <v>0.0879875818181818</v>
       </c>
       <c r="AP10">
-        <v>0.122955176470588</v>
+        <v>0.113823509090909</v>
       </c>
       <c r="AQ10">
-        <v>0.099129674</v>
+        <v>0.0918505535714285</v>
       </c>
       <c r="AR10">
-        <v>0.0956646346153846</v>
+        <v>0.0952945454545455</v>
       </c>
     </row>
   </sheetData>
@@ -1862,133 +1862,133 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.841666666666667</v>
+        <v>0.825</v>
       </c>
       <c r="C2">
+        <v>0.95</v>
+      </c>
+      <c r="D2">
+        <v>0.85</v>
+      </c>
+      <c r="E2">
+        <v>0.95</v>
+      </c>
+      <c r="F2">
+        <v>0.925</v>
+      </c>
+      <c r="G2">
+        <v>0.975</v>
+      </c>
+      <c r="H2">
+        <v>0.925</v>
+      </c>
+      <c r="I2">
+        <v>1.1</v>
+      </c>
+      <c r="J2">
+        <v>0.983333333333333</v>
+      </c>
+      <c r="K2">
+        <v>1.11666666666667</v>
+      </c>
+      <c r="L2">
+        <v>0.925</v>
+      </c>
+      <c r="M2">
+        <v>1.04166666666667</v>
+      </c>
+      <c r="N2">
+        <v>1.03333333333333</v>
+      </c>
+      <c r="O2">
+        <v>0.991666666666667</v>
+      </c>
+      <c r="P2">
+        <v>0.983333333333333</v>
+      </c>
+      <c r="Q2">
+        <v>1.06666666666667</v>
+      </c>
+      <c r="R2">
+        <v>1.00833333333333</v>
+      </c>
+      <c r="S2">
+        <v>1.11666666666667</v>
+      </c>
+      <c r="T2">
+        <v>0.958333333333333</v>
+      </c>
+      <c r="U2">
+        <v>1.00833333333333</v>
+      </c>
+      <c r="V2">
         <v>1.05</v>
       </c>
-      <c r="D2">
-        <v>0.95</v>
-      </c>
-      <c r="E2">
+      <c r="W2">
+        <v>0.933333333333333</v>
+      </c>
+      <c r="X2">
         <v>1.00833333333333</v>
       </c>
-      <c r="F2">
-        <v>0.983333333333333</v>
-      </c>
-      <c r="G2">
-        <v>1.05833333333333</v>
-      </c>
-      <c r="H2">
-        <v>1.03333333333333</v>
-      </c>
-      <c r="I2">
-        <v>1.13333333333333</v>
-      </c>
-      <c r="J2">
-        <v>1.06666666666667</v>
-      </c>
-      <c r="K2">
-        <v>1.15</v>
-      </c>
-      <c r="L2">
-        <v>1.00833333333333</v>
-      </c>
-      <c r="M2">
-        <v>1.09166666666667</v>
-      </c>
-      <c r="N2">
-        <v>1.08333333333333</v>
-      </c>
-      <c r="O2">
-        <v>1.05833333333333</v>
-      </c>
-      <c r="P2">
-        <v>1.05833333333333</v>
-      </c>
-      <c r="Q2">
-        <v>1.125</v>
-      </c>
-      <c r="R2">
-        <v>1.08333333333333</v>
-      </c>
-      <c r="S2">
-        <v>1.14166666666667</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>1.05833333333333</v>
-      </c>
-      <c r="V2">
-        <v>1.13333333333333</v>
-      </c>
-      <c r="W2">
-        <v>0.983333333333333</v>
-      </c>
-      <c r="X2">
-        <v>1.06666666666667</v>
-      </c>
       <c r="Y2">
-        <v>1.05</v>
+        <v>0.966666666666667</v>
       </c>
       <c r="Z2">
-        <v>1.075</v>
+        <v>0.975</v>
       </c>
       <c r="AA2">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="AB2">
-        <v>0.75</v>
+        <v>0.691666666666667</v>
       </c>
       <c r="AC2">
-        <v>0.683333333333333</v>
+        <v>0.616666666666667</v>
       </c>
       <c r="AD2">
-        <v>0.7</v>
+        <v>0.641666666666667</v>
       </c>
       <c r="AE2">
-        <v>0.633333333333333</v>
+        <v>0.591666666666667</v>
       </c>
       <c r="AF2">
-        <v>0.641666666666667</v>
+        <v>0.608333333333333</v>
       </c>
       <c r="AG2">
+        <v>0.591666666666667</v>
+      </c>
+      <c r="AH2">
+        <v>0.6</v>
+      </c>
+      <c r="AI2">
+        <v>0.6</v>
+      </c>
+      <c r="AJ2">
+        <v>0.566666666666667</v>
+      </c>
+      <c r="AK2">
         <v>0.608333333333333</v>
       </c>
-      <c r="AH2">
-        <v>0.641666666666667</v>
-      </c>
-      <c r="AI2">
-        <v>0.633333333333333</v>
-      </c>
-      <c r="AJ2">
+      <c r="AL2">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="AM2">
+        <v>0.566666666666667</v>
+      </c>
+      <c r="AN2">
         <v>0.616666666666667</v>
       </c>
-      <c r="AK2">
-        <v>0.65</v>
-      </c>
-      <c r="AL2">
-        <v>0.616666666666667</v>
-      </c>
-      <c r="AM2">
-        <v>0.625</v>
-      </c>
-      <c r="AN2">
-        <v>0.633333333333333</v>
-      </c>
       <c r="AO2">
-        <v>0.65</v>
+        <v>0.608333333333333</v>
       </c>
       <c r="AP2">
+        <v>0.6</v>
+      </c>
+      <c r="AQ2">
+        <v>0.6</v>
+      </c>
+      <c r="AR2">
         <v>0.608333333333333</v>
-      </c>
-      <c r="AQ2">
-        <v>0.65</v>
-      </c>
-      <c r="AR2">
-        <v>0.633333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:44">
@@ -1996,133 +1996,133 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>-2.2749807601602</v>
+        <v>-1.90553226961876</v>
       </c>
       <c r="C3">
-        <v>-2.01553910641402</v>
+        <v>-1.80353103923496</v>
       </c>
       <c r="D3">
-        <v>-1.97866569873326</v>
+        <v>-1.83587535096858</v>
       </c>
       <c r="E3">
-        <v>-1.84737432781685</v>
+        <v>-1.69752451408365</v>
       </c>
       <c r="F3">
-        <v>-2.15574780664335</v>
+        <v>-1.91244365065184</v>
       </c>
       <c r="G3">
-        <v>-1.93392833741571</v>
+        <v>-1.81595728648933</v>
       </c>
       <c r="H3">
-        <v>-2.02599088444037</v>
+        <v>-1.77092888041639</v>
       </c>
       <c r="I3">
-        <v>-2.16051651214056</v>
+        <v>-1.94198707273754</v>
       </c>
       <c r="J3">
-        <v>-2.01376187033119</v>
+        <v>-1.90786225811287</v>
       </c>
       <c r="K3">
-        <v>-1.8128754351092</v>
+        <v>-1.71057204385079</v>
       </c>
       <c r="L3">
-        <v>-2.17918867490388</v>
+        <v>-1.96724498081803</v>
       </c>
       <c r="M3">
-        <v>-1.82727986470223</v>
+        <v>-1.73226809977287</v>
       </c>
       <c r="N3">
-        <v>-1.90924164947877</v>
+        <v>-1.81364834833903</v>
       </c>
       <c r="O3">
-        <v>-2.0492869929521</v>
+        <v>-1.91831052927901</v>
       </c>
       <c r="P3">
-        <v>-2.00564635097116</v>
+        <v>-1.9390145483551</v>
       </c>
       <c r="Q3">
-        <v>-2.09322429956752</v>
+        <v>-1.95282816784062</v>
       </c>
       <c r="R3">
-        <v>-2.29382439526921</v>
+        <v>-2.07436289640254</v>
       </c>
       <c r="S3">
-        <v>-2.1975121730521</v>
+        <v>-2.00145182340904</v>
       </c>
       <c r="T3">
-        <v>-2.47785249435983</v>
+        <v>-2.27823616405595</v>
       </c>
       <c r="U3">
-        <v>-2.61896263052591</v>
+        <v>-2.40936871747602</v>
       </c>
       <c r="V3">
-        <v>-2.24365642064871</v>
+        <v>-2.09147490005899</v>
       </c>
       <c r="W3">
-        <v>-2.2798057746109</v>
+        <v>-2.00818174633214</v>
       </c>
       <c r="X3">
-        <v>-2.16280559525969</v>
+        <v>-2.02141184539895</v>
       </c>
       <c r="Y3">
-        <v>-2.46017749425481</v>
+        <v>-2.31284164374652</v>
       </c>
       <c r="Z3">
-        <v>-2.35453275918216</v>
+        <v>-2.19457082662813</v>
       </c>
       <c r="AA3">
-        <v>-3.37448842856083</v>
+        <v>-2.92821328022662</v>
       </c>
       <c r="AB3">
-        <v>-3.92271753524339</v>
+        <v>-3.36848694739665</v>
       </c>
       <c r="AC3">
-        <v>-4.63488293553073</v>
+        <v>-3.80784905171027</v>
       </c>
       <c r="AD3">
-        <v>-4.27596943251338</v>
+        <v>-3.64353703790059</v>
       </c>
       <c r="AE3">
-        <v>-4.52243690702359</v>
+        <v>-3.7706250696579</v>
       </c>
       <c r="AF3">
-        <v>-4.44448868913321</v>
+        <v>-3.79381756162199</v>
       </c>
       <c r="AG3">
-        <v>-4.87115058843218</v>
+        <v>-3.97321778048878</v>
       </c>
       <c r="AH3">
-        <v>-4.8982728301299</v>
+        <v>-4.11102245733753</v>
       </c>
       <c r="AI3">
-        <v>-4.63734179053693</v>
+        <v>-3.93822246961158</v>
       </c>
       <c r="AJ3">
-        <v>-4.77913120044251</v>
+        <v>-3.99586136983003</v>
       </c>
       <c r="AK3">
-        <v>-4.49020942989779</v>
+        <v>-3.83846370844784</v>
       </c>
       <c r="AL3">
-        <v>-4.70643233673962</v>
+        <v>-3.99480252537336</v>
       </c>
       <c r="AM3">
-        <v>-5.04051525124521</v>
+        <v>-4.24566271338047</v>
       </c>
       <c r="AN3">
-        <v>-4.48861251173522</v>
+        <v>-3.85399956825659</v>
       </c>
       <c r="AO3">
-        <v>-4.6174661883818</v>
+        <v>-3.85906588080031</v>
       </c>
       <c r="AP3">
-        <v>-4.74408297045756</v>
+        <v>-4.03112136722846</v>
       </c>
       <c r="AQ3">
-        <v>-5.14961322112459</v>
+        <v>-4.30422069956064</v>
       </c>
       <c r="AR3">
-        <v>-4.60837469917868</v>
+        <v>-3.84380880011611</v>
       </c>
     </row>
     <row r="4" spans="1:44">
@@ -2130,133 +2130,133 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>74.2574257425743</v>
+        <v>68.6868686868687</v>
       </c>
       <c r="C4">
+        <v>72.8070175438597</v>
+      </c>
+      <c r="D4">
+        <v>71.5686274509804</v>
+      </c>
+      <c r="E4">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="F4">
+        <v>73.8738738738739</v>
+      </c>
+      <c r="G4">
+        <v>80.3418803418803</v>
+      </c>
+      <c r="H4">
+        <v>45.9459459459459</v>
+      </c>
+      <c r="I4">
+        <v>75</v>
+      </c>
+      <c r="J4">
+        <v>77.1186440677966</v>
+      </c>
+      <c r="K4">
+        <v>70.8955223880597</v>
+      </c>
+      <c r="L4">
+        <v>75.6756756756757</v>
+      </c>
+      <c r="M4">
+        <v>60.8</v>
+      </c>
+      <c r="N4">
+        <v>74.1935483870968</v>
+      </c>
+      <c r="O4">
+        <v>63.0252100840336</v>
+      </c>
+      <c r="P4">
+        <v>72.8813559322034</v>
+      </c>
+      <c r="Q4">
+        <v>76.5625</v>
+      </c>
+      <c r="R4">
+        <v>69.4214876033058</v>
+      </c>
+      <c r="S4">
+        <v>74.6268656716418</v>
+      </c>
+      <c r="T4">
+        <v>72.1739130434783</v>
+      </c>
+      <c r="U4">
+        <v>73.5537190082645</v>
+      </c>
+      <c r="V4">
         <v>76.984126984127</v>
       </c>
-      <c r="D4">
-        <v>75.4385964912281</v>
-      </c>
-      <c r="E4">
-        <v>72.7272727272727</v>
-      </c>
-      <c r="F4">
-        <v>77.9661016949153</v>
-      </c>
-      <c r="G4">
-        <v>85.0393700787402</v>
-      </c>
-      <c r="H4">
-        <v>37.0967741935484</v>
-      </c>
-      <c r="I4">
-        <v>77.9411764705882</v>
-      </c>
-      <c r="J4">
-        <v>81.25</v>
-      </c>
-      <c r="K4">
-        <v>76.0869565217391</v>
-      </c>
-      <c r="L4">
-        <v>61.1570247933884</v>
-      </c>
-      <c r="M4">
-        <v>65.6488549618321</v>
-      </c>
-      <c r="N4">
-        <v>79.2307692307692</v>
-      </c>
-      <c r="O4">
-        <v>67.7165354330709</v>
-      </c>
-      <c r="P4">
-        <v>66.1417322834646</v>
-      </c>
-      <c r="Q4">
-        <v>80.7407407407407</v>
-      </c>
-      <c r="R4">
-        <v>73.8461538461539</v>
-      </c>
-      <c r="S4">
-        <v>79.5620437956204</v>
-      </c>
-      <c r="T4">
-        <v>70.8333333333333</v>
-      </c>
-      <c r="U4">
-        <v>70.8661417322835</v>
-      </c>
-      <c r="V4">
-        <v>78.6764705882353</v>
-      </c>
       <c r="W4">
-        <v>48.3050847457627</v>
+        <v>50</v>
       </c>
       <c r="X4">
-        <v>84.375</v>
+        <v>80.1652892561983</v>
       </c>
       <c r="Y4">
-        <v>74.6031746031746</v>
+        <v>80.1724137931034</v>
       </c>
       <c r="Z4">
-        <v>82.9457364341085</v>
+        <v>77.7777777777778</v>
       </c>
       <c r="AA4">
-        <v>56.25</v>
+        <v>57.7777777777778</v>
       </c>
       <c r="AB4">
-        <v>62.2222222222222</v>
+        <v>59.0361445783133</v>
       </c>
       <c r="AC4">
-        <v>63.4146341463415</v>
+        <v>55.4054054054054</v>
       </c>
       <c r="AD4">
-        <v>65.4761904761905</v>
+        <v>57.1428571428571</v>
       </c>
       <c r="AE4">
-        <v>53.9473684210526</v>
+        <v>53.5211267605634</v>
       </c>
       <c r="AF4">
-        <v>55.8441558441558</v>
+        <v>56.1643835616438</v>
       </c>
       <c r="AG4">
-        <v>52.0547945205479</v>
+        <v>53.5211267605634</v>
       </c>
       <c r="AH4">
-        <v>64.9350649350649</v>
+        <v>58.3333333333333</v>
       </c>
       <c r="AI4">
-        <v>59.2105263157895</v>
+        <v>58.3333333333333</v>
       </c>
       <c r="AJ4">
-        <v>56.7567567567568</v>
+        <v>52.9411764705882</v>
       </c>
       <c r="AK4">
-        <v>60.2564102564103</v>
+        <v>54.7945205479452</v>
       </c>
       <c r="AL4">
-        <v>40.5405405405405</v>
+        <v>55.7142857142857</v>
       </c>
       <c r="AM4">
-        <v>62.6666666666667</v>
+        <v>58.8235294117647</v>
       </c>
       <c r="AN4">
-        <v>63.1578947368421</v>
+        <v>62.1621621621622</v>
       </c>
       <c r="AO4">
-        <v>51.2820512820513</v>
+        <v>53.4246575342466</v>
       </c>
       <c r="AP4">
+        <v>55.5555555555556</v>
+      </c>
+      <c r="AQ4">
+        <v>55.5555555555556</v>
+      </c>
+      <c r="AR4">
         <v>54.7945205479452</v>
-      </c>
-      <c r="AQ4">
-        <v>53.8461538461538</v>
-      </c>
-      <c r="AR4">
-        <v>43.421052631579</v>
       </c>
     </row>
     <row r="5" spans="1:44">
@@ -2264,133 +2264,133 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>-0.924981864962263</v>
+        <v>-0.78733663990537</v>
       </c>
       <c r="C5">
-        <v>-1.03678088116649</v>
+        <v>-0.92273635037425</v>
       </c>
       <c r="D5">
-        <v>-1.14295370726069</v>
+        <v>-1.00014486316304</v>
       </c>
       <c r="E5">
-        <v>-1.20462713758439</v>
+        <v>-1.06552993868722</v>
       </c>
       <c r="F5">
-        <v>-1.32927075986062</v>
+        <v>-1.14263945207314</v>
       </c>
       <c r="G5">
-        <v>-1.42809126469166</v>
+        <v>-1.23266310291331</v>
       </c>
       <c r="H5">
-        <v>-1.43599139317632</v>
+        <v>-1.27539944815012</v>
       </c>
       <c r="I5">
-        <v>-1.58558095094726</v>
+        <v>-1.35558008506551</v>
       </c>
       <c r="J5">
-        <v>-1.46957611791622</v>
+        <v>-1.26609134899017</v>
       </c>
       <c r="K5">
-        <v>-1.45028675820602</v>
+        <v>-1.25659374195123</v>
       </c>
       <c r="L5">
-        <v>-1.48644014763487</v>
+        <v>-1.28147850528543</v>
       </c>
       <c r="M5">
-        <v>-1.52231269795777</v>
+        <v>-1.30938743568555</v>
       </c>
       <c r="N5">
-        <v>-1.53165694440383</v>
+        <v>-1.3124480673833</v>
       </c>
       <c r="O5">
-        <v>-1.50012462150966</v>
+        <v>-1.30694432380278</v>
       </c>
       <c r="P5">
-        <v>-1.53800851257562</v>
+        <v>-1.33817374194379</v>
       </c>
       <c r="Q5">
-        <v>-1.60216730297736</v>
+        <v>-1.35186521915565</v>
       </c>
       <c r="R5">
-        <v>-1.5419440597577</v>
+        <v>-1.31529780672496</v>
       </c>
       <c r="S5">
-        <v>-1.57724602117349</v>
+        <v>-1.32163909558429</v>
       </c>
       <c r="T5">
-        <v>-1.61885090489895</v>
+        <v>-1.35133248337014</v>
       </c>
       <c r="U5">
-        <v>-1.6874177861076</v>
+        <v>-1.42386654110717</v>
       </c>
       <c r="V5">
-        <v>-1.54262050380559</v>
+        <v>-1.31972711570637</v>
       </c>
       <c r="W5">
-        <v>-1.58425652543869</v>
+        <v>-1.343978257692</v>
       </c>
       <c r="X5">
-        <v>-1.68024388562854</v>
+        <v>-1.42916312756215</v>
       </c>
       <c r="Y5">
-        <v>-1.64129344564179</v>
+        <v>-1.37236747476662</v>
       </c>
       <c r="Z5">
-        <v>-1.65964708861979</v>
+        <v>-1.39177472206798</v>
       </c>
       <c r="AA5">
-        <v>-1.59879752337549</v>
+        <v>-1.30384649281848</v>
       </c>
       <c r="AB5">
-        <v>-1.70392333484024</v>
+        <v>-1.36860953419287</v>
       </c>
       <c r="AC5">
-        <v>-1.6767705235695</v>
+        <v>-1.34886366866041</v>
       </c>
       <c r="AD5">
-        <v>-1.71352038564346</v>
+        <v>-1.38818578296837</v>
       </c>
       <c r="AE5">
-        <v>-1.77494322144935</v>
+        <v>-1.41919192777315</v>
       </c>
       <c r="AF5">
-        <v>-1.87465251190944</v>
+        <v>-1.48921550811752</v>
       </c>
       <c r="AG5">
-        <v>-1.90220947809312</v>
+        <v>-1.48591293295702</v>
       </c>
       <c r="AH5">
-        <v>-1.85170460698421</v>
+        <v>-1.45534000650859</v>
       </c>
       <c r="AI5">
-        <v>-1.81947704282239</v>
+        <v>-1.43838409789831</v>
       </c>
       <c r="AJ5">
-        <v>-1.84984205061501</v>
+        <v>-1.47633203009201</v>
       </c>
       <c r="AK5">
-        <v>-1.79362148814448</v>
+        <v>-1.44003638905652</v>
       </c>
       <c r="AL5">
-        <v>-1.9457856331774</v>
+        <v>-1.54610372866334</v>
       </c>
       <c r="AM5">
-        <v>-1.89194854726217</v>
+        <v>-1.48025089380996</v>
       </c>
       <c r="AN5">
-        <v>-1.96829709589382</v>
+        <v>-1.54522410871181</v>
       </c>
       <c r="AO5">
-        <v>-1.97973526006979</v>
+        <v>-1.56951139876747</v>
       </c>
       <c r="AP5">
-        <v>-1.97855265440093</v>
+        <v>-1.56923551272064</v>
       </c>
       <c r="AQ5">
-        <v>-2.01781149701173</v>
+        <v>-1.60079328580373</v>
       </c>
       <c r="AR5">
-        <v>-2.03061547124724</v>
+        <v>-1.61854917951184</v>
       </c>
     </row>
     <row r="6" spans="1:44">
@@ -2398,133 +2398,133 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.14465537</v>
+        <v>0.151502357142857</v>
       </c>
       <c r="C6">
-        <v>0.0684581128</v>
+        <v>0.0576603911504425</v>
       </c>
       <c r="D6">
-        <v>0.103969943362832</v>
+        <v>0.100466495049505</v>
       </c>
       <c r="E6">
-        <v>0.0887125183333333</v>
+        <v>0.0786893292035398</v>
       </c>
       <c r="F6">
-        <v>0.130712406837607</v>
+        <v>0.124433151818182</v>
       </c>
       <c r="G6">
-        <v>0.126903276190476</v>
+        <v>0.126098282758621</v>
       </c>
       <c r="H6">
-        <v>0.073110756097561</v>
+        <v>0.0687238909090909</v>
       </c>
       <c r="I6">
-        <v>0.118633953333333</v>
+        <v>0.115790954198473</v>
       </c>
       <c r="J6">
-        <v>0.13386031496063</v>
+        <v>0.135152</v>
       </c>
       <c r="K6">
-        <v>0.150859372262774</v>
+        <v>0.136389676691729</v>
       </c>
       <c r="L6">
-        <v>0.0746231</v>
+        <v>0.0763792545454546</v>
       </c>
       <c r="M6">
-        <v>0.11785392</v>
+        <v>0.127212927419355</v>
       </c>
       <c r="N6">
-        <v>0.116392475968992</v>
+        <v>0.110660946341463</v>
       </c>
       <c r="O6">
-        <v>0.092114553968254</v>
+        <v>0.0812644644067797</v>
       </c>
       <c r="P6">
-        <v>0.0593325174603175</v>
+        <v>0.067924547008547</v>
       </c>
       <c r="Q6">
-        <v>0.0910869705970149</v>
+        <v>0.0849643075590551</v>
       </c>
       <c r="R6">
-        <v>0.0993918217054264</v>
+        <v>0.10676355</v>
       </c>
       <c r="S6">
-        <v>0.0803694102941176</v>
+        <v>0.0811309308270677</v>
       </c>
       <c r="T6">
-        <v>0.0992170302521008</v>
+        <v>0.0995860350877193</v>
       </c>
       <c r="U6">
-        <v>0.0908077619047619</v>
+        <v>0.0870381833333334</v>
       </c>
       <c r="V6">
-        <v>0.125711755555556</v>
+        <v>0.121121456</v>
       </c>
       <c r="W6">
-        <v>0.0800732820512821</v>
+        <v>0.086860126126126</v>
       </c>
       <c r="X6">
-        <v>0.136194692913386</v>
+        <v>0.133227308333333</v>
       </c>
       <c r="Y6">
-        <v>0.0918603216</v>
+        <v>0.0900412539130435</v>
       </c>
       <c r="Z6">
-        <v>0.099558265625</v>
+        <v>0.107828172413793</v>
       </c>
       <c r="AA6">
-        <v>0.159693684210526</v>
+        <v>0.176342426966292</v>
       </c>
       <c r="AB6">
-        <v>0.164431685393258</v>
+        <v>0.172022817073171</v>
       </c>
       <c r="AC6">
-        <v>0.0858525679012345</v>
+        <v>0.121985342465753</v>
       </c>
       <c r="AD6">
-        <v>0.206720915662651</v>
+        <v>0.202112289473684</v>
       </c>
       <c r="AE6">
-        <v>0.188692373333333</v>
+        <v>0.20665</v>
       </c>
       <c r="AF6">
-        <v>0.129170276315789</v>
+        <v>0.132123444444444</v>
       </c>
       <c r="AG6">
-        <v>0.168861608333333</v>
+        <v>0.136894368571429</v>
       </c>
       <c r="AH6">
-        <v>0.214615184210526</v>
+        <v>0.248114943661972</v>
       </c>
       <c r="AI6">
-        <v>0.19952028</v>
+        <v>0.182397352112676</v>
       </c>
       <c r="AJ6">
-        <v>0.182419082191781</v>
+        <v>0.185373074626866</v>
       </c>
       <c r="AK6">
-        <v>0.314578805194805</v>
+        <v>0.306624861111111</v>
       </c>
       <c r="AL6">
-        <v>0.320244575342466</v>
+        <v>0.317780869565217</v>
       </c>
       <c r="AM6">
-        <v>0.151854154054054</v>
+        <v>0.137292811940299</v>
       </c>
       <c r="AN6">
-        <v>0.244391552</v>
+        <v>0.258805479452055</v>
       </c>
       <c r="AO6">
-        <v>0.175572376623377</v>
+        <v>0.177700519444444</v>
       </c>
       <c r="AP6">
-        <v>0.169266416666667</v>
+        <v>0.20392523943662</v>
       </c>
       <c r="AQ6">
-        <v>0.154554038961039</v>
+        <v>0.180497563380282</v>
       </c>
       <c r="AR6">
-        <v>0.141892213333333</v>
+        <v>0.1631145</v>
       </c>
     </row>
     <row r="7" spans="1:44">
@@ -2532,133 +2532,133 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.05690767</v>
+        <v>0.0609964897959184</v>
       </c>
       <c r="C7">
-        <v>0.064981232</v>
+        <v>0.0605642654867257</v>
       </c>
       <c r="D7">
-        <v>0.0861728814159292</v>
+        <v>0.0849486396039604</v>
       </c>
       <c r="E7">
-        <v>0.147165033333333</v>
+        <v>0.146664221238938</v>
       </c>
       <c r="F7">
-        <v>0.108749128205128</v>
+        <v>0.0945577090909091</v>
       </c>
       <c r="G7">
-        <v>0.153989682539683</v>
+        <v>0.117793189655172</v>
       </c>
       <c r="H7">
-        <v>0.104984146341463</v>
+        <v>0.0726300909090909</v>
       </c>
       <c r="I7">
-        <v>0.2455408</v>
+        <v>0.211090488549618</v>
       </c>
       <c r="J7">
-        <v>0.150557637795276</v>
+        <v>0.107876068376068</v>
       </c>
       <c r="K7">
-        <v>0.146839678832117</v>
+        <v>0.113848195488722</v>
       </c>
       <c r="L7">
-        <v>0.154558</v>
+        <v>0.116861172727273</v>
       </c>
       <c r="M7">
-        <v>0.129615246153846</v>
+        <v>0.0978665483870968</v>
       </c>
       <c r="N7">
-        <v>0.209231937984496</v>
+        <v>0.180908455284553</v>
       </c>
       <c r="O7">
-        <v>0.164480317460317</v>
+        <v>0.118508957627119</v>
       </c>
       <c r="P7">
-        <v>0.14425753968254</v>
+        <v>0.100534615384615</v>
       </c>
       <c r="Q7">
-        <v>0.168911149253731</v>
+        <v>0.137327905511811</v>
       </c>
       <c r="R7">
-        <v>0.152069534883721</v>
+        <v>0.1072205</v>
       </c>
       <c r="S7">
-        <v>0.208027044117647</v>
+        <v>0.18932630075188</v>
       </c>
       <c r="T7">
-        <v>0.215588487394958</v>
+        <v>0.174906929824562</v>
       </c>
       <c r="U7">
-        <v>0.191523412698413</v>
+        <v>0.161188416666667</v>
       </c>
       <c r="V7">
-        <v>0.215225481481481</v>
+        <v>0.181552744</v>
       </c>
       <c r="W7">
-        <v>0.241977777777778</v>
+        <v>0.204142702702703</v>
       </c>
       <c r="X7">
-        <v>0.242426062992126</v>
+        <v>0.214584416666667</v>
       </c>
       <c r="Y7">
-        <v>0.20432688</v>
+        <v>0.163019568695652</v>
       </c>
       <c r="Z7">
-        <v>0.2316875</v>
+        <v>0.191305025862069</v>
       </c>
       <c r="AA7">
-        <v>0.406902315789474</v>
+        <v>0.365742134831461</v>
       </c>
       <c r="AB7">
-        <v>0.287298539325843</v>
+        <v>0.248792195121951</v>
       </c>
       <c r="AC7">
-        <v>0.281429185185185</v>
+        <v>0.242678821917808</v>
       </c>
       <c r="AD7">
-        <v>0.382710602409639</v>
+        <v>0.361101578947369</v>
       </c>
       <c r="AE7">
-        <v>0.376669386666667</v>
+        <v>0.378060485714286</v>
       </c>
       <c r="AF7">
-        <v>0.435307828947368</v>
+        <v>0.476967777777778</v>
       </c>
       <c r="AG7">
-        <v>0.502061527777778</v>
+        <v>0.549223142857143</v>
       </c>
       <c r="AH7">
-        <v>0.320338631578947</v>
+        <v>0.34543261971831</v>
       </c>
       <c r="AI7">
-        <v>0.330453093333333</v>
+        <v>0.329990028169014</v>
       </c>
       <c r="AJ7">
-        <v>0.416272301369863</v>
+        <v>0.441267611940299</v>
       </c>
       <c r="AK7">
-        <v>0.405323103896104</v>
+        <v>0.43718275</v>
       </c>
       <c r="AL7">
-        <v>0.456490612328767</v>
+        <v>0.492869275362319</v>
       </c>
       <c r="AM7">
-        <v>0.330264945945946</v>
+        <v>0.362195910447761</v>
       </c>
       <c r="AN7">
-        <v>0.4305044</v>
+        <v>0.473243287671233</v>
       </c>
       <c r="AO7">
-        <v>0.375237168831169</v>
+        <v>0.414248888888889</v>
       </c>
       <c r="AP7">
-        <v>0.454073</v>
+        <v>0.492520845070423</v>
       </c>
       <c r="AQ7">
-        <v>0.362457688311688</v>
+        <v>0.383437211267606</v>
       </c>
       <c r="AR7">
-        <v>0.39406528</v>
+        <v>0.426268972222222</v>
       </c>
     </row>
     <row r="8" spans="1:44">
@@ -2666,133 +2666,133 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>1.65918681</v>
+        <v>1.54631191836735</v>
       </c>
       <c r="C8">
-        <v>0.70580864</v>
+        <v>0.554435575221239</v>
       </c>
       <c r="D8">
-        <v>1.10994752212389</v>
+        <v>1.2005098019802</v>
       </c>
       <c r="E8">
-        <v>1.01504908333333</v>
+        <v>1.11770601769912</v>
       </c>
       <c r="F8">
-        <v>1.8676958974359</v>
+        <v>1.85558018181818</v>
       </c>
       <c r="G8">
-        <v>1.52632412698413</v>
+        <v>1.7586125862069</v>
       </c>
       <c r="H8">
-        <v>0.974007317073171</v>
+        <v>0.851639636363636</v>
       </c>
       <c r="I8">
-        <v>1.07961681481481</v>
+        <v>1.07708259541985</v>
       </c>
       <c r="J8">
-        <v>1.63774448818898</v>
+        <v>1.63390512820513</v>
       </c>
       <c r="K8">
-        <v>2.02422280291971</v>
+        <v>1.97426706766917</v>
       </c>
       <c r="L8">
-        <v>0.718920216666667</v>
+        <v>0.737331054545454</v>
       </c>
       <c r="M8">
-        <v>1.13956315384615</v>
+        <v>1.30610887096774</v>
       </c>
       <c r="N8">
-        <v>1.4541311627907</v>
+        <v>1.51482504065041</v>
       </c>
       <c r="O8">
-        <v>1.16310265079365</v>
+        <v>1.1683053559322</v>
       </c>
       <c r="P8">
-        <v>0.617049047619048</v>
+        <v>0.686584632478633</v>
       </c>
       <c r="Q8">
-        <v>1.21581564179104</v>
+        <v>1.24387366929134</v>
       </c>
       <c r="R8">
-        <v>1.30325475968992</v>
+        <v>1.40255636666667</v>
       </c>
       <c r="S8">
-        <v>1.04838044117647</v>
+        <v>1.0356777443609</v>
       </c>
       <c r="T8">
-        <v>1.0413827394958</v>
+        <v>1.10160728070175</v>
       </c>
       <c r="U8">
-        <v>0.871450703174603</v>
+        <v>0.957140405</v>
       </c>
       <c r="V8">
-        <v>1.71106554074074</v>
+        <v>1.671637264</v>
       </c>
       <c r="W8">
-        <v>0.845636076923077</v>
+        <v>0.989684504504504</v>
       </c>
       <c r="X8">
-        <v>1.4170694488189</v>
+        <v>1.52633433333333</v>
       </c>
       <c r="Y8">
-        <v>0.947498</v>
+        <v>1.02807686956522</v>
       </c>
       <c r="Z8">
-        <v>1.394875546875</v>
+        <v>1.66632543103448</v>
       </c>
       <c r="AA8">
-        <v>1.84464549473684</v>
+        <v>1.75728631460674</v>
       </c>
       <c r="AB8">
-        <v>1.88998471910112</v>
+        <v>2.11216</v>
       </c>
       <c r="AC8">
-        <v>1.24571520987654</v>
+        <v>1.33979945205479</v>
       </c>
       <c r="AD8">
-        <v>2.30967421686747</v>
+        <v>2.05970657894737</v>
       </c>
       <c r="AE8">
-        <v>3.13381466666667</v>
+        <v>3.52037185714286</v>
       </c>
       <c r="AF8">
-        <v>1.44677171052632</v>
+        <v>1.66481111111111</v>
       </c>
       <c r="AG8">
-        <v>1.7284125</v>
+        <v>1.76895714285714</v>
       </c>
       <c r="AH8">
-        <v>2.77902894736842</v>
+        <v>3.29478028169014</v>
       </c>
       <c r="AI8">
-        <v>1.73033813333333</v>
+        <v>1.95709802816901</v>
       </c>
       <c r="AJ8">
-        <v>2.19581397260274</v>
+        <v>1.87416895522388</v>
       </c>
       <c r="AK8">
-        <v>3.86898103896104</v>
+        <v>4.40178833333333</v>
       </c>
       <c r="AL8">
-        <v>4.19025767123288</v>
+        <v>4.72888772463768</v>
       </c>
       <c r="AM8">
-        <v>0.868370810810811</v>
+        <v>1.10211164179104</v>
       </c>
       <c r="AN8">
-        <v>2.5642448</v>
+        <v>3.0112095890411</v>
       </c>
       <c r="AO8">
-        <v>2.04804454545454</v>
+        <v>2.41000611111111</v>
       </c>
       <c r="AP8">
-        <v>2.56507972222222</v>
+        <v>2.77225563380282</v>
       </c>
       <c r="AQ8">
-        <v>1.79627701298701</v>
+        <v>2.28685225352113</v>
       </c>
       <c r="AR8">
-        <v>2.18220773333333</v>
+        <v>2.00574861111111</v>
       </c>
     </row>
     <row r="9" spans="1:44">
@@ -2800,133 +2800,133 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.0467612</v>
+        <v>0.0488497959183673</v>
       </c>
       <c r="C9">
-        <v>0.036962256</v>
+        <v>0.0377379380530973</v>
       </c>
       <c r="D9">
-        <v>0.0551941061946903</v>
+        <v>0.0440375247524753</v>
       </c>
       <c r="E9">
-        <v>0.0413194583333334</v>
+        <v>0.0423816814159292</v>
       </c>
       <c r="F9">
-        <v>0.0510235726495727</v>
+        <v>0.0560161818181818</v>
       </c>
       <c r="G9">
-        <v>0.0339340793650794</v>
+        <v>0.0342457896551724</v>
       </c>
       <c r="H9">
-        <v>0.0290951707317073</v>
+        <v>0.0267998181818182</v>
       </c>
       <c r="I9">
-        <v>0.0273085407407408</v>
+        <v>0.0270881603053435</v>
       </c>
       <c r="J9">
-        <v>0.0372654251968504</v>
+        <v>0.0340768205128205</v>
       </c>
       <c r="K9">
-        <v>0.0442293284671533</v>
+        <v>0.0397135864661654</v>
       </c>
       <c r="L9">
-        <v>0.0285582833333333</v>
+        <v>0.0310244181818182</v>
       </c>
       <c r="M9">
-        <v>0.0351605230769231</v>
+        <v>0.0352497419354839</v>
       </c>
       <c r="N9">
-        <v>0.0242389069767442</v>
+        <v>0.0243866910569106</v>
       </c>
       <c r="O9">
-        <v>0.0349419682539683</v>
+        <v>0.0319362118644068</v>
       </c>
       <c r="P9">
-        <v>0.0299833174603175</v>
+        <v>0.0339379572649573</v>
       </c>
       <c r="Q9">
-        <v>0.0381271864925373</v>
+        <v>0.0405501811023622</v>
       </c>
       <c r="R9">
-        <v>0.0315459069767442</v>
+        <v>0.03153441</v>
       </c>
       <c r="S9">
-        <v>0.0413335441176471</v>
+        <v>0.0447114318045113</v>
       </c>
       <c r="T9">
-        <v>0.0418230588235294</v>
+        <v>0.0410815614035088</v>
       </c>
       <c r="U9">
-        <v>0.0303691428571429</v>
+        <v>0.0290946666666667</v>
       </c>
       <c r="V9">
-        <v>0.0701694666666667</v>
+        <v>0.061168448</v>
       </c>
       <c r="W9">
-        <v>0.0404164273504274</v>
+        <v>0.0415961261261261</v>
       </c>
       <c r="X9">
-        <v>0.0473149511811023</v>
+        <v>0.0472582816666667</v>
       </c>
       <c r="Y9">
-        <v>0.0256943704</v>
+        <v>0.0285081913043478</v>
       </c>
       <c r="Z9">
-        <v>0.032875984375</v>
+        <v>0.0343295172413793</v>
       </c>
       <c r="AA9">
-        <v>0.0691081473684211</v>
+        <v>0.0622957528089888</v>
       </c>
       <c r="AB9">
-        <v>0.0574467865168539</v>
+        <v>0.0587216829268293</v>
       </c>
       <c r="AC9">
-        <v>0.0838848148148148</v>
+        <v>0.0869986301369862</v>
       </c>
       <c r="AD9">
-        <v>0.0884321397590361</v>
+        <v>0.0891013421052631</v>
       </c>
       <c r="AE9">
-        <v>0.126408</v>
+        <v>0.122799142857143</v>
       </c>
       <c r="AF9">
-        <v>0.102102631578947</v>
+        <v>0.0993704166666667</v>
       </c>
       <c r="AG9">
-        <v>0.0911965416666667</v>
+        <v>0.101940857142857</v>
       </c>
       <c r="AH9">
-        <v>0.0838201052631579</v>
+        <v>0.0962155352112676</v>
       </c>
       <c r="AI9">
-        <v>0.0645721333333333</v>
+        <v>0.0749448450704226</v>
       </c>
       <c r="AJ9">
-        <v>0.075852506849315</v>
+        <v>0.0686688358208955</v>
       </c>
       <c r="AK9">
-        <v>0.104815363636364</v>
+        <v>0.108745111111111</v>
       </c>
       <c r="AL9">
-        <v>0.147192164383562</v>
+        <v>0.121664536231884</v>
       </c>
       <c r="AM9">
-        <v>0.114487635135135</v>
+        <v>0.096659104477612</v>
       </c>
       <c r="AN9">
-        <v>0.069682368</v>
+        <v>0.0651959808219178</v>
       </c>
       <c r="AO9">
-        <v>0.0743960649350649</v>
+        <v>0.0773584583333333</v>
       </c>
       <c r="AP9">
-        <v>0.0976620625</v>
+        <v>0.100659394366197</v>
       </c>
       <c r="AQ9">
-        <v>0.0679662077922078</v>
+        <v>0.0727487323943662</v>
       </c>
       <c r="AR9">
-        <v>0.0877056</v>
+        <v>0.0889732222222222</v>
       </c>
     </row>
   </sheetData>
@@ -3211,13 +3211,13 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>-2.49804</v>
+        <v>-2.6609</v>
       </c>
       <c r="C3">
-        <v>-2.94278</v>
+        <v>-2.9934</v>
       </c>
       <c r="D3">
-        <v>-2.9934</v>
+        <v>-3.63156</v>
       </c>
       <c r="E3">
         <v>-4.0067</v>
@@ -3241,7 +3241,7 @@
         <v>-3.97499</v>
       </c>
       <c r="L3">
-        <v>-3.15265</v>
+        <v>-3.65271</v>
       </c>
       <c r="M3">
         <v>-4.16679</v>
@@ -3253,7 +3253,7 @@
         <v>-3.9661</v>
       </c>
       <c r="P3">
-        <v>-3.40628</v>
+        <v>-3.91619</v>
       </c>
       <c r="Q3">
         <v>-4.19485</v>
@@ -3271,7 +3271,7 @@
         <v>-3.47256</v>
       </c>
       <c r="V3">
-        <v>-3.56835</v>
+        <v>-4.34919</v>
       </c>
       <c r="W3">
         <v>-4.67316</v>
@@ -3289,10 +3289,10 @@
         <v>-6.6904</v>
       </c>
       <c r="AB3">
-        <v>-6.39995</v>
+        <v>-5.73102</v>
       </c>
       <c r="AC3">
-        <v>-5.73102</v>
+        <v>-5.72732</v>
       </c>
       <c r="AD3">
         <v>-6.74113</v>
@@ -3345,133 +3345,133 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.125519113861386</v>
+        <v>0.131513428571429</v>
       </c>
       <c r="C4">
-        <v>0.103088060576923</v>
+        <v>0.0948962913461538</v>
       </c>
       <c r="D4">
-        <v>0.108553188043478</v>
+        <v>0.109992738378378</v>
       </c>
       <c r="E4">
-        <v>0.100033354871795</v>
+        <v>0.100154739487179</v>
       </c>
       <c r="F4">
-        <v>0.158650448351648</v>
+        <v>0.159849375409836</v>
       </c>
       <c r="G4">
-        <v>0.126002431351351</v>
+        <v>0.126574611290323</v>
       </c>
       <c r="H4">
-        <v>0.127738952380952</v>
+        <v>0.126862603174603</v>
       </c>
       <c r="I4">
-        <v>0.136374312565445</v>
+        <v>0.13702081025641</v>
       </c>
       <c r="J4">
-        <v>0.148030560209424</v>
+        <v>0.153102389473684</v>
       </c>
       <c r="K4">
-        <v>0.172655479591837</v>
+        <v>0.167445414141414</v>
       </c>
       <c r="L4">
-        <v>0.100161158469945</v>
+        <v>0.0993730601092896</v>
       </c>
       <c r="M4">
-        <v>0.133378274468085</v>
+        <v>0.136580610582011</v>
       </c>
       <c r="N4">
-        <v>0.134808480434783</v>
+        <v>0.130472647311828</v>
       </c>
       <c r="O4">
-        <v>0.107186052406417</v>
+        <v>0.106625635294118</v>
       </c>
       <c r="P4">
-        <v>0.0991846909090909</v>
+        <v>0.104534914893617</v>
       </c>
       <c r="Q4">
-        <v>0.109072089789474</v>
+        <v>0.103180131204188</v>
       </c>
       <c r="R4">
-        <v>0.0977941189189189</v>
+        <v>0.101149016042781</v>
       </c>
       <c r="S4">
-        <v>0.105452623958333</v>
+        <v>0.101666693264249</v>
       </c>
       <c r="T4">
-        <v>0.106897725287356</v>
+        <v>0.108264264</v>
       </c>
       <c r="U4">
-        <v>0.128704688888889</v>
+        <v>0.127986519337017</v>
       </c>
       <c r="V4">
-        <v>0.144241300518135</v>
+        <v>0.147251445595855</v>
       </c>
       <c r="W4">
-        <v>0.119027867052023</v>
+        <v>0.120731873563218</v>
       </c>
       <c r="X4">
-        <v>0.163815934426229</v>
+        <v>0.161198184782609</v>
       </c>
       <c r="Y4">
-        <v>0.134411006741573</v>
+        <v>0.133535140782123</v>
       </c>
       <c r="Z4">
-        <v>0.119253910614525</v>
+        <v>0.123673372222222</v>
       </c>
       <c r="AA4">
-        <v>0.265164797297297</v>
+        <v>0.266687526666667</v>
       </c>
       <c r="AB4">
-        <v>0.237327157142857</v>
+        <v>0.240859971428571</v>
       </c>
       <c r="AC4">
-        <v>0.190666770992366</v>
+        <v>0.19416647368421</v>
       </c>
       <c r="AD4">
-        <v>0.293455656716418</v>
+        <v>0.283515691176471</v>
       </c>
       <c r="AE4">
-        <v>0.250488417322835</v>
+        <v>0.250000236220472</v>
       </c>
       <c r="AF4">
-        <v>0.185411086614173</v>
+        <v>0.191116828125</v>
       </c>
       <c r="AG4">
-        <v>0.234116457377049</v>
+        <v>0.218848925203252</v>
       </c>
       <c r="AH4">
-        <v>0.185462274193548</v>
+        <v>0.20547988</v>
       </c>
       <c r="AI4">
-        <v>0.317007588709677</v>
+        <v>0.303886341269841</v>
       </c>
       <c r="AJ4">
-        <v>0.230575443548387</v>
+        <v>0.23171964516129</v>
       </c>
       <c r="AK4">
-        <v>0.307115515873016</v>
+        <v>0.319041984251968</v>
       </c>
       <c r="AL4">
-        <v>0.376025170731708</v>
+        <v>0.376056325203252</v>
       </c>
       <c r="AM4">
-        <v>0.232681961666667</v>
+        <v>0.230939027868853</v>
       </c>
       <c r="AN4">
-        <v>0.2309213328</v>
+        <v>0.234547719047619</v>
       </c>
       <c r="AO4">
-        <v>0.231062875</v>
+        <v>0.22502990625</v>
       </c>
       <c r="AP4">
-        <v>0.263093</v>
+        <v>0.272376236220473</v>
       </c>
       <c r="AQ4">
-        <v>0.21286003125</v>
+        <v>0.214008171875</v>
       </c>
       <c r="AR4">
-        <v>0.2033122421875</v>
+        <v>0.209427609375</v>
       </c>
     </row>
     <row r="5" spans="1:44">
@@ -3479,133 +3479,133 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.0468991386138614</v>
+        <v>0.0462325911330049</v>
       </c>
       <c r="C5">
-        <v>0.0841923846153846</v>
+        <v>0.0834463269230769</v>
       </c>
       <c r="D5">
-        <v>0.119917916304348</v>
+        <v>0.124245170810811</v>
       </c>
       <c r="E5">
-        <v>0.189979558974359</v>
+        <v>0.187567046153846</v>
       </c>
       <c r="F5">
-        <v>0.158438615384615</v>
+        <v>0.161026</v>
       </c>
       <c r="G5">
-        <v>0.195428756756757</v>
+        <v>0.19336935483871</v>
       </c>
       <c r="H5">
-        <v>0.160081534391534</v>
+        <v>0.160221164021164</v>
       </c>
       <c r="I5">
-        <v>0.251632816753927</v>
+        <v>0.249136656410256</v>
       </c>
       <c r="J5">
-        <v>0.178879267015707</v>
+        <v>0.177786736842105</v>
       </c>
       <c r="K5">
-        <v>0.175493295918367</v>
+        <v>0.172864525252525</v>
       </c>
       <c r="L5">
-        <v>0.172138415300546</v>
+        <v>0.175879180327869</v>
       </c>
       <c r="M5">
-        <v>0.16964064893617</v>
+        <v>0.168222920634921</v>
       </c>
       <c r="N5">
-        <v>0.220022608695652</v>
+        <v>0.221325</v>
       </c>
       <c r="O5">
-        <v>0.201567112299465</v>
+        <v>0.198636042780749</v>
       </c>
       <c r="P5">
-        <v>0.180781764705882</v>
+        <v>0.181993617021277</v>
       </c>
       <c r="Q5">
-        <v>0.197785494736842</v>
+        <v>0.198693162303665</v>
       </c>
       <c r="R5">
-        <v>0.191144486486486</v>
+        <v>0.188761604278075</v>
       </c>
       <c r="S5">
-        <v>0.217463010416667</v>
+        <v>0.218228694300518</v>
       </c>
       <c r="T5">
-        <v>0.231009252873563</v>
+        <v>0.226295542857143</v>
       </c>
       <c r="U5">
-        <v>0.202265722222222</v>
+        <v>0.204099171270718</v>
       </c>
       <c r="V5">
-        <v>0.230176062176166</v>
+        <v>0.231150259067358</v>
       </c>
       <c r="W5">
-        <v>0.256084335260115</v>
+        <v>0.255387873563218</v>
       </c>
       <c r="X5">
-        <v>0.249228469945355</v>
+        <v>0.250572717391304</v>
       </c>
       <c r="Y5">
-        <v>0.229698258426966</v>
+        <v>0.228870893854749</v>
       </c>
       <c r="Z5">
-        <v>0.251906368715084</v>
+        <v>0.251356722222222</v>
       </c>
       <c r="AA5">
-        <v>0.3848175</v>
+        <v>0.380751133333333</v>
       </c>
       <c r="AB5">
-        <v>0.296050285714286</v>
+        <v>0.2907435</v>
       </c>
       <c r="AC5">
-        <v>0.295990259541985</v>
+        <v>0.299167097744361</v>
       </c>
       <c r="AD5">
-        <v>0.375430373134328</v>
+        <v>0.379208897058823</v>
       </c>
       <c r="AE5">
-        <v>0.379222157480315</v>
+        <v>0.38373137007874</v>
       </c>
       <c r="AF5">
-        <v>0.43116468503937</v>
+        <v>0.4406434375</v>
       </c>
       <c r="AG5">
-        <v>0.494885549180328</v>
+        <v>0.495543170731707</v>
       </c>
       <c r="AH5">
-        <v>0.365189048387097</v>
+        <v>0.354249408</v>
       </c>
       <c r="AI5">
-        <v>0.346427032258064</v>
+        <v>0.344441126984127</v>
       </c>
       <c r="AJ5">
-        <v>0.39719014516129</v>
+        <v>0.404951935483871</v>
       </c>
       <c r="AK5">
-        <v>0.412170738095238</v>
+        <v>0.405580062992126</v>
       </c>
       <c r="AL5">
-        <v>0.425661639837398</v>
+        <v>0.430277804878049</v>
       </c>
       <c r="AM5">
-        <v>0.361777491666667</v>
+        <v>0.357507098360656</v>
       </c>
       <c r="AN5">
-        <v>0.42305656</v>
+        <v>0.433013968253968</v>
       </c>
       <c r="AO5">
-        <v>0.39850509375</v>
+        <v>0.39403140625</v>
       </c>
       <c r="AP5">
-        <v>0.427665532258064</v>
+        <v>0.423982204724409</v>
       </c>
       <c r="AQ5">
-        <v>0.3738114453125</v>
+        <v>0.36711259375</v>
       </c>
       <c r="AR5">
-        <v>0.37084809375</v>
+        <v>0.3770523125</v>
       </c>
     </row>
     <row r="6" spans="1:44">
@@ -3613,133 +3613,133 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.34590539603961</v>
+        <v>1.37698220689655</v>
       </c>
       <c r="C6">
-        <v>1.11456383653846</v>
+        <v>1.096416875</v>
       </c>
       <c r="D6">
-        <v>1.2070539673913</v>
+        <v>1.23761664864865</v>
       </c>
       <c r="E6">
-        <v>1.08686574358974</v>
+        <v>1.12329948717949</v>
       </c>
       <c r="F6">
-        <v>2.26500164835165</v>
+        <v>2.18844054644809</v>
       </c>
       <c r="G6">
-        <v>1.41962140540541</v>
+        <v>1.56937612903226</v>
       </c>
       <c r="H6">
-        <v>1.40276439153439</v>
+        <v>1.33859502645503</v>
       </c>
       <c r="I6">
-        <v>1.40608994764398</v>
+        <v>1.37590861538461</v>
       </c>
       <c r="J6">
-        <v>1.77440654450262</v>
+        <v>1.84537</v>
       </c>
       <c r="K6">
-        <v>1.99993428571429</v>
+        <v>1.98822535353535</v>
       </c>
       <c r="L6">
-        <v>0.918924295081967</v>
+        <v>0.910646644808743</v>
       </c>
       <c r="M6">
-        <v>1.32568003191489</v>
+        <v>1.35666291005291</v>
       </c>
       <c r="N6">
-        <v>1.78648983695652</v>
+        <v>1.74872596774193</v>
       </c>
       <c r="O6">
-        <v>1.21207782887701</v>
+        <v>1.23350027807487</v>
       </c>
       <c r="P6">
-        <v>1.20696497326203</v>
+        <v>1.19495107446809</v>
       </c>
       <c r="Q6">
-        <v>1.53635261052632</v>
+        <v>1.50734468062827</v>
       </c>
       <c r="R6">
-        <v>1.31491418378378</v>
+        <v>1.33864451336898</v>
       </c>
       <c r="S6">
-        <v>1.34423666666667</v>
+        <v>1.2945525388601</v>
       </c>
       <c r="T6">
-        <v>1.03791965517241</v>
+        <v>1.07559382857143</v>
       </c>
       <c r="U6">
-        <v>1.43376921444444</v>
+        <v>1.44892004751381</v>
       </c>
       <c r="V6">
-        <v>1.78626366839378</v>
+        <v>1.77813035233161</v>
       </c>
       <c r="W6">
-        <v>1.28901341040462</v>
+        <v>1.37673954022988</v>
       </c>
       <c r="X6">
-        <v>1.85826043715847</v>
+        <v>1.85008836956522</v>
       </c>
       <c r="Y6">
-        <v>1.32041169662921</v>
+        <v>1.28700705027933</v>
       </c>
       <c r="Z6">
-        <v>1.47381117318436</v>
+        <v>1.60201277777778</v>
       </c>
       <c r="AA6">
-        <v>3.0316992027027</v>
+        <v>2.90808054666667</v>
       </c>
       <c r="AB6">
-        <v>2.46344828571429</v>
+        <v>2.51315828571429</v>
       </c>
       <c r="AC6">
-        <v>2.13294717557252</v>
+        <v>2.07500571428571</v>
       </c>
       <c r="AD6">
-        <v>3.16974223880597</v>
+        <v>3.31283691176471</v>
       </c>
       <c r="AE6">
-        <v>3.31086354330709</v>
+        <v>3.33553409448819</v>
       </c>
       <c r="AF6">
-        <v>2.27734606299212</v>
+        <v>2.248757578125</v>
       </c>
       <c r="AG6">
-        <v>2.51820176229508</v>
+        <v>2.42356520325203</v>
       </c>
       <c r="AH6">
-        <v>2.37497</v>
+        <v>2.46009904</v>
       </c>
       <c r="AI6">
-        <v>3.18731580645161</v>
+        <v>3.21424968253968</v>
       </c>
       <c r="AJ6">
-        <v>2.71955096774193</v>
+        <v>2.60488</v>
       </c>
       <c r="AK6">
-        <v>3.48105761904762</v>
+        <v>3.65264637795275</v>
       </c>
       <c r="AL6">
-        <v>4.0178037398374</v>
+        <v>3.98390555284553</v>
       </c>
       <c r="AM6">
-        <v>1.939297</v>
+        <v>1.88146087704918</v>
       </c>
       <c r="AN6">
-        <v>2.26485732</v>
+        <v>2.40916206349206</v>
       </c>
       <c r="AO6">
-        <v>2.64803265625</v>
+        <v>2.56689390625</v>
       </c>
       <c r="AP6">
-        <v>3.39890887096774</v>
+        <v>3.3825342519685</v>
       </c>
       <c r="AQ6">
-        <v>2.4806665625</v>
+        <v>2.44935234375</v>
       </c>
       <c r="AR6">
-        <v>2.6950046875</v>
+        <v>2.533391171875</v>
       </c>
     </row>
     <row r="7" spans="1:44">
@@ -3747,133 +3747,133 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.0532841089108911</v>
+        <v>0.0551775862068966</v>
       </c>
       <c r="C7">
-        <v>0.0488360961538462</v>
+        <v>0.0472371057692308</v>
       </c>
       <c r="D7">
-        <v>0.0612385</v>
+        <v>0.0604305081081081</v>
       </c>
       <c r="E7">
-        <v>0.053886441025641</v>
+        <v>0.0543223897435898</v>
       </c>
       <c r="F7">
-        <v>0.063908</v>
+        <v>0.066039868852459</v>
       </c>
       <c r="G7">
-        <v>0.0418061513513514</v>
+        <v>0.0409397903225806</v>
       </c>
       <c r="H7">
-        <v>0.0384878201058201</v>
+        <v>0.0370530793650794</v>
       </c>
       <c r="I7">
-        <v>0.043499832460733</v>
+        <v>0.043680517948718</v>
       </c>
       <c r="J7">
-        <v>0.056136392670157</v>
+        <v>0.0559939842105263</v>
       </c>
       <c r="K7">
-        <v>0.0505104693877551</v>
+        <v>0.0499359595959596</v>
       </c>
       <c r="L7">
-        <v>0.0413393442622951</v>
+        <v>0.0413751038251366</v>
       </c>
       <c r="M7">
-        <v>0.0433326489361702</v>
+        <v>0.0437360211640212</v>
       </c>
       <c r="N7">
-        <v>0.0361221032608696</v>
+        <v>0.0367552580645161</v>
       </c>
       <c r="O7">
-        <v>0.0496505882352941</v>
+        <v>0.0491350267379679</v>
       </c>
       <c r="P7">
-        <v>0.0538709411764706</v>
+        <v>0.054828</v>
       </c>
       <c r="Q7">
-        <v>0.0496387578421053</v>
+        <v>0.0502914345549738</v>
       </c>
       <c r="R7">
-        <v>0.0513672394594594</v>
+        <v>0.0509093112299465</v>
       </c>
       <c r="S7">
-        <v>0.0536434010416667</v>
+        <v>0.054807695492228</v>
       </c>
       <c r="T7">
-        <v>0.0501633793103448</v>
+        <v>0.0492195975428571</v>
       </c>
       <c r="U7">
-        <v>0.0500900777777778</v>
+        <v>0.0488195248618784</v>
       </c>
       <c r="V7">
-        <v>0.0863205077720207</v>
+        <v>0.0869712849740932</v>
       </c>
       <c r="W7">
-        <v>0.0532785664739884</v>
+        <v>0.0518405862068965</v>
       </c>
       <c r="X7">
-        <v>0.0595294524590164</v>
+        <v>0.0586600532608695</v>
       </c>
       <c r="Y7">
-        <v>0.0393274044943821</v>
+        <v>0.0412109385474861</v>
       </c>
       <c r="Z7">
-        <v>0.0420346145251396</v>
+        <v>0.0404982</v>
       </c>
       <c r="AA7">
-        <v>0.0888322594594595</v>
+        <v>0.0905904293333333</v>
       </c>
       <c r="AB7">
-        <v>0.0731692428571429</v>
+        <v>0.0707427428571429</v>
       </c>
       <c r="AC7">
-        <v>0.0930672977099236</v>
+        <v>0.094434932330827</v>
       </c>
       <c r="AD7">
-        <v>0.0999079671641791</v>
+        <v>0.0999764529411765</v>
       </c>
       <c r="AE7">
-        <v>0.106105354330709</v>
+        <v>0.103585039370079</v>
       </c>
       <c r="AF7">
-        <v>0.104650787401575</v>
+        <v>0.105510625</v>
       </c>
       <c r="AG7">
-        <v>0.104830662295082</v>
+        <v>0.111224152845528</v>
       </c>
       <c r="AH7">
-        <v>0.0918372580645161</v>
+        <v>0.089353224</v>
       </c>
       <c r="AI7">
-        <v>0.0923108709677419</v>
+        <v>0.0908957857142857</v>
       </c>
       <c r="AJ7">
-        <v>0.0964681693548387</v>
+        <v>0.0956670322580645</v>
       </c>
       <c r="AK7">
-        <v>0.121913904761905</v>
+        <v>0.12131725984252</v>
       </c>
       <c r="AL7">
-        <v>0.170440707317073</v>
+        <v>0.169855520325203</v>
       </c>
       <c r="AM7">
-        <v>0.131875808333333</v>
+        <v>0.130916057377049</v>
       </c>
       <c r="AN7">
-        <v>0.0853143008</v>
+        <v>0.0835200603174603</v>
       </c>
       <c r="AO7">
-        <v>0.0804033359375</v>
+        <v>0.0819153046875001</v>
       </c>
       <c r="AP7">
-        <v>0.107396826612903</v>
+        <v>0.106665826771654</v>
       </c>
       <c r="AQ7">
-        <v>0.07974485703125</v>
+        <v>0.0806116484375</v>
       </c>
       <c r="AR7">
-        <v>0.0905198515625</v>
+        <v>0.0921318125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>